<commit_message>
+ BGU-16 Basic desktop applications UI for questionnaires filling : roughly done
</commit_message>
<xml_diff>
--- a/BGU.DRPL.SignificantOwnership/Codegen/BGU_xsd_outil16.xlsx
+++ b/BGU.DRPL.SignificantOwnership/Codegen/BGU_xsd_outil16.xlsx
@@ -9,11 +9,12 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9915" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9915" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Forms" sheetId="2" r:id="rId2"/>
+    <sheet name="TypeEditors" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="50">
   <si>
     <t>ClassName</t>
   </si>
@@ -124,6 +125,57 @@
   </si>
   <si>
     <t>ModalForm</t>
+  </si>
+  <si>
+    <t>RegLicAppx14NewSvc</t>
+  </si>
+  <si>
+    <t>RegLicAppx2LPQuest</t>
+  </si>
+  <si>
+    <t>RegLicAppx4PhysPQuest</t>
+  </si>
+  <si>
+    <t>RegLicAppx7ShareAcqIntent</t>
+  </si>
+  <si>
+    <t>AttachmentInfo</t>
+  </si>
+  <si>
+    <t>BankingLicensedActivityInfo</t>
+  </si>
+  <si>
+    <t>BankingLicenseInfo</t>
+  </si>
+  <si>
+    <t>ContactInfo</t>
+  </si>
+  <si>
+    <t>CouncilMemberInfo</t>
+  </si>
+  <si>
+    <t>CurrencyAmount</t>
+  </si>
+  <si>
+    <t>GenericPersonID</t>
+  </si>
+  <si>
+    <t>GenericPersonIDShare</t>
+  </si>
+  <si>
+    <t>GenericPersonInfo</t>
+  </si>
+  <si>
+    <t>OwnershipStructure</t>
+  </si>
+  <si>
+    <t>PersonsAssociation</t>
+  </si>
+  <si>
+    <t>PhoneInfo</t>
+  </si>
+  <si>
+    <t>PurchasedVoteInfo</t>
   </si>
 </sst>
 </file>
@@ -775,7 +827,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
@@ -934,4 +986,1203 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:I32"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="I32" sqref="I32"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" t="str">
+        <f>"I"&amp; TRIM(A1) &amp; "EditFormFactory"</f>
+        <v>IAppx2OwnershipStructLPEditFormFactory</v>
+      </c>
+      <c r="C1" t="str">
+        <f>"public interface " &amp; B1 &amp; " : ITypeEditorFormFactoryBase { }"</f>
+        <v>public interface IAppx2OwnershipStructLPEditFormFactory : ITypeEditorFormFactoryBase { }</v>
+      </c>
+      <c r="D1" t="str">
+        <f>A1&amp; "_Editor"</f>
+        <v>Appx2OwnershipStructLP_Editor</v>
+      </c>
+      <c r="E1" t="str">
+        <f>"public class " &amp; D1 &amp; " : GenericTypeEditor&lt;"&amp;A1&amp;"&gt; { private " &amp; B1 &amp; " _fact; protected override ITypeEditorFormFactoryBase TypeEditorFormFactory { get { if (_fact == null) _fact = TypeEditorsDispatcher.Container.Resolve&lt;" &amp;B1 &amp; "&gt;(); return _fact; } }  }"</f>
+        <v>public class Appx2OwnershipStructLP_Editor : GenericTypeEditor&lt;Appx2OwnershipStructLP&gt; { private IAppx2OwnershipStructLPEditFormFactory _fact; protected override ITypeEditorFormFactoryBase TypeEditorFormFactory { get { if (_fact == null) _fact = TypeEditorsDispatcher.Container.Resolve&lt;IAppx2OwnershipStructLPEditFormFactory&gt;(); return _fact; } }  }</v>
+      </c>
+      <c r="F1" t="str">
+        <f>A1&amp; "EditFormFactoryBasic"</f>
+        <v>Appx2OwnershipStructLPEditFormFactoryBasic</v>
+      </c>
+      <c r="G1" t="str">
+        <f>"public class " &amp;F1&amp; " : " &amp; B1 &amp; " { public System.Windows.Forms.Form SpawnInstance() { return new DummyForm&lt;" &amp;A1&amp; " &gt;(); } }"</f>
+        <v>public class Appx2OwnershipStructLPEditFormFactoryBasic : IAppx2OwnershipStructLPEditFormFactory { public System.Windows.Forms.Form SpawnInstance() { return new DummyForm&lt;Appx2OwnershipStructLP &gt;(); } }</v>
+      </c>
+      <c r="H1" t="str">
+        <f>"cont.RegisterInstance&lt;" &amp; B1 &amp; "&gt;(new " &amp; F1 &amp; "(), new ContainerControlledLifetimeManager());"</f>
+        <v>cont.RegisterInstance&lt;IAppx2OwnershipStructLPEditFormFactory&gt;(new Appx2OwnershipStructLPEditFormFactoryBasic(), new ContainerControlledLifetimeManager());</v>
+      </c>
+      <c r="I1" t="str">
+        <f>"[System.ComponentModel.Editor(typeof(BGU.DRPL.SignificantOwnership.Core.TypeEditors." &amp;D1 &amp; "), typeof(System.Drawing.Design.UITypeEditor))]"</f>
+        <v>[System.ComponentModel.Editor(typeof(BGU.DRPL.SignificantOwnership.Core.TypeEditors.Appx2OwnershipStructLP_Editor), typeof(System.Drawing.Design.UITypeEditor))]</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B2" t="str">
+        <f t="shared" ref="B2:B32" si="0">"I"&amp; TRIM(A2) &amp; "EditFormFactory"</f>
+        <v>IRegLicAppx14NewSvcEditFormFactory</v>
+      </c>
+      <c r="C2" t="str">
+        <f t="shared" ref="C2:C32" si="1">"public interface I"&amp; TRIM(A2) &amp; "EditFormFactory : ITypeEditorFormFactoryBase { }"</f>
+        <v>public interface IRegLicAppx14NewSvcEditFormFactory : ITypeEditorFormFactoryBase { }</v>
+      </c>
+      <c r="D2" t="str">
+        <f t="shared" ref="D2:D32" si="2">A2&amp; "_Editor"</f>
+        <v>RegLicAppx14NewSvc_Editor</v>
+      </c>
+      <c r="E2" t="str">
+        <f t="shared" ref="E2:E32" si="3">"public class " &amp; D2 &amp; " : GenericTypeEditor&lt;"&amp;A2&amp;"&gt; { private " &amp; B2 &amp; " _fact; protected override ITypeEditorFormFactoryBase TypeEditorFormFactory { get { if (_fact == null) _fact = TypeEditorsDispatcher.Container.Resolve&lt;" &amp;B2 &amp; "&gt;(); return _fact; } }  }"</f>
+        <v>public class RegLicAppx14NewSvc_Editor : GenericTypeEditor&lt;RegLicAppx14NewSvc&gt; { private IRegLicAppx14NewSvcEditFormFactory _fact; protected override ITypeEditorFormFactoryBase TypeEditorFormFactory { get { if (_fact == null) _fact = TypeEditorsDispatcher.Container.Resolve&lt;IRegLicAppx14NewSvcEditFormFactory&gt;(); return _fact; } }  }</v>
+      </c>
+      <c r="F2" t="str">
+        <f t="shared" ref="F2:F32" si="4">A2&amp; "EditFormFactoryBasic"</f>
+        <v>RegLicAppx14NewSvcEditFormFactoryBasic</v>
+      </c>
+      <c r="G2" t="str">
+        <f t="shared" ref="G2:G32" si="5">"public class " &amp;F2&amp; " : " &amp; B2 &amp; " { public System.Windows.Forms.Form SpawnInstance() { return new DummyForm&lt;" &amp;A2&amp; " &gt;(); } }"</f>
+        <v>public class RegLicAppx14NewSvcEditFormFactoryBasic : IRegLicAppx14NewSvcEditFormFactory { public System.Windows.Forms.Form SpawnInstance() { return new DummyForm&lt;RegLicAppx14NewSvc &gt;(); } }</v>
+      </c>
+      <c r="H2" t="str">
+        <f t="shared" ref="H2:H32" si="6">"cont.RegisterInstance&lt;" &amp; B2 &amp; "&gt;(new " &amp; F2 &amp; "(), new ContainerControlledLifetimeManager());"</f>
+        <v>cont.RegisterInstance&lt;IRegLicAppx14NewSvcEditFormFactory&gt;(new RegLicAppx14NewSvcEditFormFactoryBasic(), new ContainerControlledLifetimeManager());</v>
+      </c>
+      <c r="I2" t="str">
+        <f t="shared" ref="I2:I32" si="7">"[System.ComponentModel.Editor(typeof(BGU.DRPL.SignificantOwnership.Core.TypeEditors." &amp;D2 &amp; "), typeof(System.Drawing.Design.UITypeEditor))]"</f>
+        <v>[System.ComponentModel.Editor(typeof(BGU.DRPL.SignificantOwnership.Core.TypeEditors.RegLicAppx14NewSvc_Editor), typeof(System.Drawing.Design.UITypeEditor))]</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>34</v>
+      </c>
+      <c r="B3" t="str">
+        <f t="shared" si="0"/>
+        <v>IRegLicAppx2LPQuestEditFormFactory</v>
+      </c>
+      <c r="C3" t="str">
+        <f t="shared" si="1"/>
+        <v>public interface IRegLicAppx2LPQuestEditFormFactory : ITypeEditorFormFactoryBase { }</v>
+      </c>
+      <c r="D3" t="str">
+        <f t="shared" si="2"/>
+        <v>RegLicAppx2LPQuest_Editor</v>
+      </c>
+      <c r="E3" t="str">
+        <f t="shared" si="3"/>
+        <v>public class RegLicAppx2LPQuest_Editor : GenericTypeEditor&lt;RegLicAppx2LPQuest&gt; { private IRegLicAppx2LPQuestEditFormFactory _fact; protected override ITypeEditorFormFactoryBase TypeEditorFormFactory { get { if (_fact == null) _fact = TypeEditorsDispatcher.Container.Resolve&lt;IRegLicAppx2LPQuestEditFormFactory&gt;(); return _fact; } }  }</v>
+      </c>
+      <c r="F3" t="str">
+        <f t="shared" si="4"/>
+        <v>RegLicAppx2LPQuestEditFormFactoryBasic</v>
+      </c>
+      <c r="G3" t="str">
+        <f t="shared" si="5"/>
+        <v>public class RegLicAppx2LPQuestEditFormFactoryBasic : IRegLicAppx2LPQuestEditFormFactory { public System.Windows.Forms.Form SpawnInstance() { return new DummyForm&lt;RegLicAppx2LPQuest &gt;(); } }</v>
+      </c>
+      <c r="H3" t="str">
+        <f t="shared" si="6"/>
+        <v>cont.RegisterInstance&lt;IRegLicAppx2LPQuestEditFormFactory&gt;(new RegLicAppx2LPQuestEditFormFactoryBasic(), new ContainerControlledLifetimeManager());</v>
+      </c>
+      <c r="I3" t="str">
+        <f t="shared" si="7"/>
+        <v>[System.ComponentModel.Editor(typeof(BGU.DRPL.SignificantOwnership.Core.TypeEditors.RegLicAppx2LPQuest_Editor), typeof(System.Drawing.Design.UITypeEditor))]</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>35</v>
+      </c>
+      <c r="B4" t="str">
+        <f t="shared" si="0"/>
+        <v>IRegLicAppx4PhysPQuestEditFormFactory</v>
+      </c>
+      <c r="C4" t="str">
+        <f t="shared" si="1"/>
+        <v>public interface IRegLicAppx4PhysPQuestEditFormFactory : ITypeEditorFormFactoryBase { }</v>
+      </c>
+      <c r="D4" t="str">
+        <f t="shared" si="2"/>
+        <v>RegLicAppx4PhysPQuest_Editor</v>
+      </c>
+      <c r="E4" t="str">
+        <f t="shared" si="3"/>
+        <v>public class RegLicAppx4PhysPQuest_Editor : GenericTypeEditor&lt;RegLicAppx4PhysPQuest&gt; { private IRegLicAppx4PhysPQuestEditFormFactory _fact; protected override ITypeEditorFormFactoryBase TypeEditorFormFactory { get { if (_fact == null) _fact = TypeEditorsDispatcher.Container.Resolve&lt;IRegLicAppx4PhysPQuestEditFormFactory&gt;(); return _fact; } }  }</v>
+      </c>
+      <c r="F4" t="str">
+        <f t="shared" si="4"/>
+        <v>RegLicAppx4PhysPQuestEditFormFactoryBasic</v>
+      </c>
+      <c r="G4" t="str">
+        <f t="shared" si="5"/>
+        <v>public class RegLicAppx4PhysPQuestEditFormFactoryBasic : IRegLicAppx4PhysPQuestEditFormFactory { public System.Windows.Forms.Form SpawnInstance() { return new DummyForm&lt;RegLicAppx4PhysPQuest &gt;(); } }</v>
+      </c>
+      <c r="H4" t="str">
+        <f t="shared" si="6"/>
+        <v>cont.RegisterInstance&lt;IRegLicAppx4PhysPQuestEditFormFactory&gt;(new RegLicAppx4PhysPQuestEditFormFactoryBasic(), new ContainerControlledLifetimeManager());</v>
+      </c>
+      <c r="I4" t="str">
+        <f t="shared" si="7"/>
+        <v>[System.ComponentModel.Editor(typeof(BGU.DRPL.SignificantOwnership.Core.TypeEditors.RegLicAppx4PhysPQuest_Editor), typeof(System.Drawing.Design.UITypeEditor))]</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>36</v>
+      </c>
+      <c r="B5" t="str">
+        <f t="shared" si="0"/>
+        <v>IRegLicAppx7ShareAcqIntentEditFormFactory</v>
+      </c>
+      <c r="C5" t="str">
+        <f t="shared" si="1"/>
+        <v>public interface IRegLicAppx7ShareAcqIntentEditFormFactory : ITypeEditorFormFactoryBase { }</v>
+      </c>
+      <c r="D5" t="str">
+        <f t="shared" si="2"/>
+        <v>RegLicAppx7ShareAcqIntent_Editor</v>
+      </c>
+      <c r="E5" t="str">
+        <f t="shared" si="3"/>
+        <v>public class RegLicAppx7ShareAcqIntent_Editor : GenericTypeEditor&lt;RegLicAppx7ShareAcqIntent&gt; { private IRegLicAppx7ShareAcqIntentEditFormFactory _fact; protected override ITypeEditorFormFactoryBase TypeEditorFormFactory { get { if (_fact == null) _fact = TypeEditorsDispatcher.Container.Resolve&lt;IRegLicAppx7ShareAcqIntentEditFormFactory&gt;(); return _fact; } }  }</v>
+      </c>
+      <c r="F5" t="str">
+        <f t="shared" si="4"/>
+        <v>RegLicAppx7ShareAcqIntentEditFormFactoryBasic</v>
+      </c>
+      <c r="G5" t="str">
+        <f t="shared" si="5"/>
+        <v>public class RegLicAppx7ShareAcqIntentEditFormFactoryBasic : IRegLicAppx7ShareAcqIntentEditFormFactory { public System.Windows.Forms.Form SpawnInstance() { return new DummyForm&lt;RegLicAppx7ShareAcqIntent &gt;(); } }</v>
+      </c>
+      <c r="H5" t="str">
+        <f t="shared" si="6"/>
+        <v>cont.RegisterInstance&lt;IRegLicAppx7ShareAcqIntentEditFormFactory&gt;(new RegLicAppx7ShareAcqIntentEditFormFactoryBasic(), new ContainerControlledLifetimeManager());</v>
+      </c>
+      <c r="I5" t="str">
+        <f t="shared" si="7"/>
+        <v>[System.ComponentModel.Editor(typeof(BGU.DRPL.SignificantOwnership.Core.TypeEditors.RegLicAppx7ShareAcqIntent_Editor), typeof(System.Drawing.Design.UITypeEditor))]</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>37</v>
+      </c>
+      <c r="B6" t="str">
+        <f t="shared" si="0"/>
+        <v>IAttachmentInfoEditFormFactory</v>
+      </c>
+      <c r="C6" t="str">
+        <f t="shared" si="1"/>
+        <v>public interface IAttachmentInfoEditFormFactory : ITypeEditorFormFactoryBase { }</v>
+      </c>
+      <c r="D6" t="str">
+        <f t="shared" si="2"/>
+        <v>AttachmentInfo_Editor</v>
+      </c>
+      <c r="E6" t="str">
+        <f t="shared" si="3"/>
+        <v>public class AttachmentInfo_Editor : GenericTypeEditor&lt;AttachmentInfo&gt; { private IAttachmentInfoEditFormFactory _fact; protected override ITypeEditorFormFactoryBase TypeEditorFormFactory { get { if (_fact == null) _fact = TypeEditorsDispatcher.Container.Resolve&lt;IAttachmentInfoEditFormFactory&gt;(); return _fact; } }  }</v>
+      </c>
+      <c r="F6" t="str">
+        <f t="shared" si="4"/>
+        <v>AttachmentInfoEditFormFactoryBasic</v>
+      </c>
+      <c r="G6" t="str">
+        <f t="shared" si="5"/>
+        <v>public class AttachmentInfoEditFormFactoryBasic : IAttachmentInfoEditFormFactory { public System.Windows.Forms.Form SpawnInstance() { return new DummyForm&lt;AttachmentInfo &gt;(); } }</v>
+      </c>
+      <c r="H6" t="str">
+        <f t="shared" si="6"/>
+        <v>cont.RegisterInstance&lt;IAttachmentInfoEditFormFactory&gt;(new AttachmentInfoEditFormFactoryBasic(), new ContainerControlledLifetimeManager());</v>
+      </c>
+      <c r="I6" t="str">
+        <f t="shared" si="7"/>
+        <v>[System.ComponentModel.Editor(typeof(BGU.DRPL.SignificantOwnership.Core.TypeEditors.AttachmentInfo_Editor), typeof(System.Drawing.Design.UITypeEditor))]</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>38</v>
+      </c>
+      <c r="B7" t="str">
+        <f t="shared" si="0"/>
+        <v>IBankingLicensedActivityInfoEditFormFactory</v>
+      </c>
+      <c r="C7" t="str">
+        <f t="shared" si="1"/>
+        <v>public interface IBankingLicensedActivityInfoEditFormFactory : ITypeEditorFormFactoryBase { }</v>
+      </c>
+      <c r="D7" t="str">
+        <f t="shared" si="2"/>
+        <v>BankingLicensedActivityInfo_Editor</v>
+      </c>
+      <c r="E7" t="str">
+        <f t="shared" si="3"/>
+        <v>public class BankingLicensedActivityInfo_Editor : GenericTypeEditor&lt;BankingLicensedActivityInfo&gt; { private IBankingLicensedActivityInfoEditFormFactory _fact; protected override ITypeEditorFormFactoryBase TypeEditorFormFactory { get { if (_fact == null) _fact = TypeEditorsDispatcher.Container.Resolve&lt;IBankingLicensedActivityInfoEditFormFactory&gt;(); return _fact; } }  }</v>
+      </c>
+      <c r="F7" t="str">
+        <f t="shared" si="4"/>
+        <v>BankingLicensedActivityInfoEditFormFactoryBasic</v>
+      </c>
+      <c r="G7" t="str">
+        <f t="shared" si="5"/>
+        <v>public class BankingLicensedActivityInfoEditFormFactoryBasic : IBankingLicensedActivityInfoEditFormFactory { public System.Windows.Forms.Form SpawnInstance() { return new DummyForm&lt;BankingLicensedActivityInfo &gt;(); } }</v>
+      </c>
+      <c r="H7" t="str">
+        <f t="shared" si="6"/>
+        <v>cont.RegisterInstance&lt;IBankingLicensedActivityInfoEditFormFactory&gt;(new BankingLicensedActivityInfoEditFormFactoryBasic(), new ContainerControlledLifetimeManager());</v>
+      </c>
+      <c r="I7" t="str">
+        <f t="shared" si="7"/>
+        <v>[System.ComponentModel.Editor(typeof(BGU.DRPL.SignificantOwnership.Core.TypeEditors.BankingLicensedActivityInfo_Editor), typeof(System.Drawing.Design.UITypeEditor))]</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>39</v>
+      </c>
+      <c r="B8" t="str">
+        <f t="shared" si="0"/>
+        <v>IBankingLicenseInfoEditFormFactory</v>
+      </c>
+      <c r="C8" t="str">
+        <f t="shared" si="1"/>
+        <v>public interface IBankingLicenseInfoEditFormFactory : ITypeEditorFormFactoryBase { }</v>
+      </c>
+      <c r="D8" t="str">
+        <f t="shared" si="2"/>
+        <v>BankingLicenseInfo_Editor</v>
+      </c>
+      <c r="E8" t="str">
+        <f t="shared" si="3"/>
+        <v>public class BankingLicenseInfo_Editor : GenericTypeEditor&lt;BankingLicenseInfo&gt; { private IBankingLicenseInfoEditFormFactory _fact; protected override ITypeEditorFormFactoryBase TypeEditorFormFactory { get { if (_fact == null) _fact = TypeEditorsDispatcher.Container.Resolve&lt;IBankingLicenseInfoEditFormFactory&gt;(); return _fact; } }  }</v>
+      </c>
+      <c r="F8" t="str">
+        <f t="shared" si="4"/>
+        <v>BankingLicenseInfoEditFormFactoryBasic</v>
+      </c>
+      <c r="G8" t="str">
+        <f t="shared" si="5"/>
+        <v>public class BankingLicenseInfoEditFormFactoryBasic : IBankingLicenseInfoEditFormFactory { public System.Windows.Forms.Form SpawnInstance() { return new DummyForm&lt;BankingLicenseInfo &gt;(); } }</v>
+      </c>
+      <c r="H8" t="str">
+        <f t="shared" si="6"/>
+        <v>cont.RegisterInstance&lt;IBankingLicenseInfoEditFormFactory&gt;(new BankingLicenseInfoEditFormFactoryBasic(), new ContainerControlledLifetimeManager());</v>
+      </c>
+      <c r="I8" t="str">
+        <f t="shared" si="7"/>
+        <v>[System.ComponentModel.Editor(typeof(BGU.DRPL.SignificantOwnership.Core.TypeEditors.BankingLicenseInfo_Editor), typeof(System.Drawing.Design.UITypeEditor))]</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>7</v>
+      </c>
+      <c r="B9" t="str">
+        <f t="shared" si="0"/>
+        <v>ICommonOwnershipInfoEditFormFactory</v>
+      </c>
+      <c r="C9" t="str">
+        <f t="shared" si="1"/>
+        <v>public interface ICommonOwnershipInfoEditFormFactory : ITypeEditorFormFactoryBase { }</v>
+      </c>
+      <c r="D9" t="str">
+        <f t="shared" si="2"/>
+        <v>CommonOwnershipInfo_Editor</v>
+      </c>
+      <c r="E9" t="str">
+        <f t="shared" si="3"/>
+        <v>public class CommonOwnershipInfo_Editor : GenericTypeEditor&lt;CommonOwnershipInfo&gt; { private ICommonOwnershipInfoEditFormFactory _fact; protected override ITypeEditorFormFactoryBase TypeEditorFormFactory { get { if (_fact == null) _fact = TypeEditorsDispatcher.Container.Resolve&lt;ICommonOwnershipInfoEditFormFactory&gt;(); return _fact; } }  }</v>
+      </c>
+      <c r="F9" t="str">
+        <f t="shared" si="4"/>
+        <v>CommonOwnershipInfoEditFormFactoryBasic</v>
+      </c>
+      <c r="G9" t="str">
+        <f t="shared" si="5"/>
+        <v>public class CommonOwnershipInfoEditFormFactoryBasic : ICommonOwnershipInfoEditFormFactory { public System.Windows.Forms.Form SpawnInstance() { return new DummyForm&lt;CommonOwnershipInfo &gt;(); } }</v>
+      </c>
+      <c r="H9" t="str">
+        <f t="shared" si="6"/>
+        <v>cont.RegisterInstance&lt;ICommonOwnershipInfoEditFormFactory&gt;(new CommonOwnershipInfoEditFormFactoryBasic(), new ContainerControlledLifetimeManager());</v>
+      </c>
+      <c r="I9" t="str">
+        <f t="shared" si="7"/>
+        <v>[System.ComponentModel.Editor(typeof(BGU.DRPL.SignificantOwnership.Core.TypeEditors.CommonOwnershipInfo_Editor), typeof(System.Drawing.Design.UITypeEditor))]</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>40</v>
+      </c>
+      <c r="B10" t="str">
+        <f t="shared" si="0"/>
+        <v>IContactInfoEditFormFactory</v>
+      </c>
+      <c r="C10" t="str">
+        <f t="shared" si="1"/>
+        <v>public interface IContactInfoEditFormFactory : ITypeEditorFormFactoryBase { }</v>
+      </c>
+      <c r="D10" t="str">
+        <f t="shared" si="2"/>
+        <v>ContactInfo_Editor</v>
+      </c>
+      <c r="E10" t="str">
+        <f t="shared" si="3"/>
+        <v>public class ContactInfo_Editor : GenericTypeEditor&lt;ContactInfo&gt; { private IContactInfoEditFormFactory _fact; protected override ITypeEditorFormFactoryBase TypeEditorFormFactory { get { if (_fact == null) _fact = TypeEditorsDispatcher.Container.Resolve&lt;IContactInfoEditFormFactory&gt;(); return _fact; } }  }</v>
+      </c>
+      <c r="F10" t="str">
+        <f t="shared" si="4"/>
+        <v>ContactInfoEditFormFactoryBasic</v>
+      </c>
+      <c r="G10" t="str">
+        <f t="shared" si="5"/>
+        <v>public class ContactInfoEditFormFactoryBasic : IContactInfoEditFormFactory { public System.Windows.Forms.Form SpawnInstance() { return new DummyForm&lt;ContactInfo &gt;(); } }</v>
+      </c>
+      <c r="H10" t="str">
+        <f t="shared" si="6"/>
+        <v>cont.RegisterInstance&lt;IContactInfoEditFormFactory&gt;(new ContactInfoEditFormFactoryBasic(), new ContainerControlledLifetimeManager());</v>
+      </c>
+      <c r="I10" t="str">
+        <f t="shared" si="7"/>
+        <v>[System.ComponentModel.Editor(typeof(BGU.DRPL.SignificantOwnership.Core.TypeEditors.ContactInfo_Editor), typeof(System.Drawing.Design.UITypeEditor))]</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>8</v>
+      </c>
+      <c r="B11" t="str">
+        <f t="shared" si="0"/>
+        <v>ICouncilBodyInfoEditFormFactory</v>
+      </c>
+      <c r="C11" t="str">
+        <f t="shared" si="1"/>
+        <v>public interface ICouncilBodyInfoEditFormFactory : ITypeEditorFormFactoryBase { }</v>
+      </c>
+      <c r="D11" t="str">
+        <f t="shared" si="2"/>
+        <v>CouncilBodyInfo_Editor</v>
+      </c>
+      <c r="E11" t="str">
+        <f t="shared" si="3"/>
+        <v>public class CouncilBodyInfo_Editor : GenericTypeEditor&lt;CouncilBodyInfo&gt; { private ICouncilBodyInfoEditFormFactory _fact; protected override ITypeEditorFormFactoryBase TypeEditorFormFactory { get { if (_fact == null) _fact = TypeEditorsDispatcher.Container.Resolve&lt;ICouncilBodyInfoEditFormFactory&gt;(); return _fact; } }  }</v>
+      </c>
+      <c r="F11" t="str">
+        <f t="shared" si="4"/>
+        <v>CouncilBodyInfoEditFormFactoryBasic</v>
+      </c>
+      <c r="G11" t="str">
+        <f t="shared" si="5"/>
+        <v>public class CouncilBodyInfoEditFormFactoryBasic : ICouncilBodyInfoEditFormFactory { public System.Windows.Forms.Form SpawnInstance() { return new DummyForm&lt;CouncilBodyInfo &gt;(); } }</v>
+      </c>
+      <c r="H11" t="str">
+        <f t="shared" si="6"/>
+        <v>cont.RegisterInstance&lt;ICouncilBodyInfoEditFormFactory&gt;(new CouncilBodyInfoEditFormFactoryBasic(), new ContainerControlledLifetimeManager());</v>
+      </c>
+      <c r="I11" t="str">
+        <f t="shared" si="7"/>
+        <v>[System.ComponentModel.Editor(typeof(BGU.DRPL.SignificantOwnership.Core.TypeEditors.CouncilBodyInfo_Editor), typeof(System.Drawing.Design.UITypeEditor))]</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>41</v>
+      </c>
+      <c r="B12" t="str">
+        <f t="shared" si="0"/>
+        <v>ICouncilMemberInfoEditFormFactory</v>
+      </c>
+      <c r="C12" t="str">
+        <f t="shared" si="1"/>
+        <v>public interface ICouncilMemberInfoEditFormFactory : ITypeEditorFormFactoryBase { }</v>
+      </c>
+      <c r="D12" t="str">
+        <f t="shared" si="2"/>
+        <v>CouncilMemberInfo_Editor</v>
+      </c>
+      <c r="E12" t="str">
+        <f t="shared" si="3"/>
+        <v>public class CouncilMemberInfo_Editor : GenericTypeEditor&lt;CouncilMemberInfo&gt; { private ICouncilMemberInfoEditFormFactory _fact; protected override ITypeEditorFormFactoryBase TypeEditorFormFactory { get { if (_fact == null) _fact = TypeEditorsDispatcher.Container.Resolve&lt;ICouncilMemberInfoEditFormFactory&gt;(); return _fact; } }  }</v>
+      </c>
+      <c r="F12" t="str">
+        <f t="shared" si="4"/>
+        <v>CouncilMemberInfoEditFormFactoryBasic</v>
+      </c>
+      <c r="G12" t="str">
+        <f t="shared" si="5"/>
+        <v>public class CouncilMemberInfoEditFormFactoryBasic : ICouncilMemberInfoEditFormFactory { public System.Windows.Forms.Form SpawnInstance() { return new DummyForm&lt;CouncilMemberInfo &gt;(); } }</v>
+      </c>
+      <c r="H12" t="str">
+        <f t="shared" si="6"/>
+        <v>cont.RegisterInstance&lt;ICouncilMemberInfoEditFormFactory&gt;(new CouncilMemberInfoEditFormFactoryBasic(), new ContainerControlledLifetimeManager());</v>
+      </c>
+      <c r="I12" t="str">
+        <f t="shared" si="7"/>
+        <v>[System.ComponentModel.Editor(typeof(BGU.DRPL.SignificantOwnership.Core.TypeEditors.CouncilMemberInfo_Editor), typeof(System.Drawing.Design.UITypeEditor))]</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>42</v>
+      </c>
+      <c r="B13" t="str">
+        <f t="shared" si="0"/>
+        <v>ICurrencyAmountEditFormFactory</v>
+      </c>
+      <c r="C13" t="str">
+        <f t="shared" si="1"/>
+        <v>public interface ICurrencyAmountEditFormFactory : ITypeEditorFormFactoryBase { }</v>
+      </c>
+      <c r="D13" t="str">
+        <f t="shared" si="2"/>
+        <v>CurrencyAmount_Editor</v>
+      </c>
+      <c r="E13" t="str">
+        <f t="shared" si="3"/>
+        <v>public class CurrencyAmount_Editor : GenericTypeEditor&lt;CurrencyAmount&gt; { private ICurrencyAmountEditFormFactory _fact; protected override ITypeEditorFormFactoryBase TypeEditorFormFactory { get { if (_fact == null) _fact = TypeEditorsDispatcher.Container.Resolve&lt;ICurrencyAmountEditFormFactory&gt;(); return _fact; } }  }</v>
+      </c>
+      <c r="F13" t="str">
+        <f t="shared" si="4"/>
+        <v>CurrencyAmountEditFormFactoryBasic</v>
+      </c>
+      <c r="G13" t="str">
+        <f t="shared" si="5"/>
+        <v>public class CurrencyAmountEditFormFactoryBasic : ICurrencyAmountEditFormFactory { public System.Windows.Forms.Form SpawnInstance() { return new DummyForm&lt;CurrencyAmount &gt;(); } }</v>
+      </c>
+      <c r="H13" t="str">
+        <f t="shared" si="6"/>
+        <v>cont.RegisterInstance&lt;ICurrencyAmountEditFormFactory&gt;(new CurrencyAmountEditFormFactoryBasic(), new ContainerControlledLifetimeManager());</v>
+      </c>
+      <c r="I13" t="str">
+        <f t="shared" si="7"/>
+        <v>[System.ComponentModel.Editor(typeof(BGU.DRPL.SignificantOwnership.Core.TypeEditors.CurrencyAmount_Editor), typeof(System.Drawing.Design.UITypeEditor))]</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>43</v>
+      </c>
+      <c r="B14" t="str">
+        <f t="shared" si="0"/>
+        <v>IGenericPersonIDEditFormFactory</v>
+      </c>
+      <c r="C14" t="str">
+        <f t="shared" si="1"/>
+        <v>public interface IGenericPersonIDEditFormFactory : ITypeEditorFormFactoryBase { }</v>
+      </c>
+      <c r="D14" t="str">
+        <f t="shared" si="2"/>
+        <v>GenericPersonID_Editor</v>
+      </c>
+      <c r="E14" t="str">
+        <f t="shared" si="3"/>
+        <v>public class GenericPersonID_Editor : GenericTypeEditor&lt;GenericPersonID&gt; { private IGenericPersonIDEditFormFactory _fact; protected override ITypeEditorFormFactoryBase TypeEditorFormFactory { get { if (_fact == null) _fact = TypeEditorsDispatcher.Container.Resolve&lt;IGenericPersonIDEditFormFactory&gt;(); return _fact; } }  }</v>
+      </c>
+      <c r="F14" t="str">
+        <f t="shared" si="4"/>
+        <v>GenericPersonIDEditFormFactoryBasic</v>
+      </c>
+      <c r="G14" t="str">
+        <f t="shared" si="5"/>
+        <v>public class GenericPersonIDEditFormFactoryBasic : IGenericPersonIDEditFormFactory { public System.Windows.Forms.Form SpawnInstance() { return new DummyForm&lt;GenericPersonID &gt;(); } }</v>
+      </c>
+      <c r="H14" t="str">
+        <f t="shared" si="6"/>
+        <v>cont.RegisterInstance&lt;IGenericPersonIDEditFormFactory&gt;(new GenericPersonIDEditFormFactoryBasic(), new ContainerControlledLifetimeManager());</v>
+      </c>
+      <c r="I14" t="str">
+        <f t="shared" si="7"/>
+        <v>[System.ComponentModel.Editor(typeof(BGU.DRPL.SignificantOwnership.Core.TypeEditors.GenericPersonID_Editor), typeof(System.Drawing.Design.UITypeEditor))]</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>44</v>
+      </c>
+      <c r="B15" t="str">
+        <f t="shared" si="0"/>
+        <v>IGenericPersonIDShareEditFormFactory</v>
+      </c>
+      <c r="C15" t="str">
+        <f t="shared" si="1"/>
+        <v>public interface IGenericPersonIDShareEditFormFactory : ITypeEditorFormFactoryBase { }</v>
+      </c>
+      <c r="D15" t="str">
+        <f t="shared" si="2"/>
+        <v>GenericPersonIDShare_Editor</v>
+      </c>
+      <c r="E15" t="str">
+        <f t="shared" si="3"/>
+        <v>public class GenericPersonIDShare_Editor : GenericTypeEditor&lt;GenericPersonIDShare&gt; { private IGenericPersonIDShareEditFormFactory _fact; protected override ITypeEditorFormFactoryBase TypeEditorFormFactory { get { if (_fact == null) _fact = TypeEditorsDispatcher.Container.Resolve&lt;IGenericPersonIDShareEditFormFactory&gt;(); return _fact; } }  }</v>
+      </c>
+      <c r="F15" t="str">
+        <f t="shared" si="4"/>
+        <v>GenericPersonIDShareEditFormFactoryBasic</v>
+      </c>
+      <c r="G15" t="str">
+        <f t="shared" si="5"/>
+        <v>public class GenericPersonIDShareEditFormFactoryBasic : IGenericPersonIDShareEditFormFactory { public System.Windows.Forms.Form SpawnInstance() { return new DummyForm&lt;GenericPersonIDShare &gt;(); } }</v>
+      </c>
+      <c r="H15" t="str">
+        <f t="shared" si="6"/>
+        <v>cont.RegisterInstance&lt;IGenericPersonIDShareEditFormFactory&gt;(new GenericPersonIDShareEditFormFactoryBasic(), new ContainerControlledLifetimeManager());</v>
+      </c>
+      <c r="I15" t="str">
+        <f t="shared" si="7"/>
+        <v>[System.ComponentModel.Editor(typeof(BGU.DRPL.SignificantOwnership.Core.TypeEditors.GenericPersonIDShare_Editor), typeof(System.Drawing.Design.UITypeEditor))]</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>45</v>
+      </c>
+      <c r="B16" t="str">
+        <f t="shared" si="0"/>
+        <v>IGenericPersonInfoEditFormFactory</v>
+      </c>
+      <c r="C16" t="str">
+        <f t="shared" si="1"/>
+        <v>public interface IGenericPersonInfoEditFormFactory : ITypeEditorFormFactoryBase { }</v>
+      </c>
+      <c r="D16" t="str">
+        <f t="shared" si="2"/>
+        <v>GenericPersonInfo_Editor</v>
+      </c>
+      <c r="E16" t="str">
+        <f t="shared" si="3"/>
+        <v>public class GenericPersonInfo_Editor : GenericTypeEditor&lt;GenericPersonInfo&gt; { private IGenericPersonInfoEditFormFactory _fact; protected override ITypeEditorFormFactoryBase TypeEditorFormFactory { get { if (_fact == null) _fact = TypeEditorsDispatcher.Container.Resolve&lt;IGenericPersonInfoEditFormFactory&gt;(); return _fact; } }  }</v>
+      </c>
+      <c r="F16" t="str">
+        <f t="shared" si="4"/>
+        <v>GenericPersonInfoEditFormFactoryBasic</v>
+      </c>
+      <c r="G16" t="str">
+        <f t="shared" si="5"/>
+        <v>public class GenericPersonInfoEditFormFactoryBasic : IGenericPersonInfoEditFormFactory { public System.Windows.Forms.Form SpawnInstance() { return new DummyForm&lt;GenericPersonInfo &gt;(); } }</v>
+      </c>
+      <c r="H16" t="str">
+        <f t="shared" si="6"/>
+        <v>cont.RegisterInstance&lt;IGenericPersonInfoEditFormFactory&gt;(new GenericPersonInfoEditFormFactoryBasic(), new ContainerControlledLifetimeManager());</v>
+      </c>
+      <c r="I16" t="str">
+        <f t="shared" si="7"/>
+        <v>[System.ComponentModel.Editor(typeof(BGU.DRPL.SignificantOwnership.Core.TypeEditors.GenericPersonInfo_Editor), typeof(System.Drawing.Design.UITypeEditor))]</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>11</v>
+      </c>
+      <c r="B17" t="str">
+        <f t="shared" si="0"/>
+        <v>ILegalPersonShareInfoEditFormFactory</v>
+      </c>
+      <c r="C17" t="str">
+        <f t="shared" si="1"/>
+        <v>public interface ILegalPersonShareInfoEditFormFactory : ITypeEditorFormFactoryBase { }</v>
+      </c>
+      <c r="D17" t="str">
+        <f t="shared" si="2"/>
+        <v>LegalPersonShareInfo_Editor</v>
+      </c>
+      <c r="E17" t="str">
+        <f t="shared" si="3"/>
+        <v>public class LegalPersonShareInfo_Editor : GenericTypeEditor&lt;LegalPersonShareInfo&gt; { private ILegalPersonShareInfoEditFormFactory _fact; protected override ITypeEditorFormFactoryBase TypeEditorFormFactory { get { if (_fact == null) _fact = TypeEditorsDispatcher.Container.Resolve&lt;ILegalPersonShareInfoEditFormFactory&gt;(); return _fact; } }  }</v>
+      </c>
+      <c r="F17" t="str">
+        <f t="shared" si="4"/>
+        <v>LegalPersonShareInfoEditFormFactoryBasic</v>
+      </c>
+      <c r="G17" t="str">
+        <f t="shared" si="5"/>
+        <v>public class LegalPersonShareInfoEditFormFactoryBasic : ILegalPersonShareInfoEditFormFactory { public System.Windows.Forms.Form SpawnInstance() { return new DummyForm&lt;LegalPersonShareInfo &gt;(); } }</v>
+      </c>
+      <c r="H17" t="str">
+        <f t="shared" si="6"/>
+        <v>cont.RegisterInstance&lt;ILegalPersonShareInfoEditFormFactory&gt;(new LegalPersonShareInfoEditFormFactoryBasic(), new ContainerControlledLifetimeManager());</v>
+      </c>
+      <c r="I17" t="str">
+        <f t="shared" si="7"/>
+        <v>[System.ComponentModel.Editor(typeof(BGU.DRPL.SignificantOwnership.Core.TypeEditors.LegalPersonShareInfo_Editor), typeof(System.Drawing.Design.UITypeEditor))]</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>46</v>
+      </c>
+      <c r="B18" t="str">
+        <f t="shared" si="0"/>
+        <v>IOwnershipStructureEditFormFactory</v>
+      </c>
+      <c r="C18" t="str">
+        <f t="shared" si="1"/>
+        <v>public interface IOwnershipStructureEditFormFactory : ITypeEditorFormFactoryBase { }</v>
+      </c>
+      <c r="D18" t="str">
+        <f t="shared" si="2"/>
+        <v>OwnershipStructure_Editor</v>
+      </c>
+      <c r="E18" t="str">
+        <f t="shared" si="3"/>
+        <v>public class OwnershipStructure_Editor : GenericTypeEditor&lt;OwnershipStructure&gt; { private IOwnershipStructureEditFormFactory _fact; protected override ITypeEditorFormFactoryBase TypeEditorFormFactory { get { if (_fact == null) _fact = TypeEditorsDispatcher.Container.Resolve&lt;IOwnershipStructureEditFormFactory&gt;(); return _fact; } }  }</v>
+      </c>
+      <c r="F18" t="str">
+        <f t="shared" si="4"/>
+        <v>OwnershipStructureEditFormFactoryBasic</v>
+      </c>
+      <c r="G18" t="str">
+        <f t="shared" si="5"/>
+        <v>public class OwnershipStructureEditFormFactoryBasic : IOwnershipStructureEditFormFactory { public System.Windows.Forms.Form SpawnInstance() { return new DummyForm&lt;OwnershipStructure &gt;(); } }</v>
+      </c>
+      <c r="H18" t="str">
+        <f t="shared" si="6"/>
+        <v>cont.RegisterInstance&lt;IOwnershipStructureEditFormFactory&gt;(new OwnershipStructureEditFormFactoryBasic(), new ContainerControlledLifetimeManager());</v>
+      </c>
+      <c r="I18" t="str">
+        <f t="shared" si="7"/>
+        <v>[System.ComponentModel.Editor(typeof(BGU.DRPL.SignificantOwnership.Core.TypeEditors.OwnershipStructure_Editor), typeof(System.Drawing.Design.UITypeEditor))]</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>12</v>
+      </c>
+      <c r="B19" t="str">
+        <f t="shared" si="0"/>
+        <v>IOwnershipSummaryInfoEditFormFactory</v>
+      </c>
+      <c r="C19" t="str">
+        <f t="shared" si="1"/>
+        <v>public interface IOwnershipSummaryInfoEditFormFactory : ITypeEditorFormFactoryBase { }</v>
+      </c>
+      <c r="D19" t="str">
+        <f t="shared" si="2"/>
+        <v>OwnershipSummaryInfo_Editor</v>
+      </c>
+      <c r="E19" t="str">
+        <f t="shared" si="3"/>
+        <v>public class OwnershipSummaryInfo_Editor : GenericTypeEditor&lt;OwnershipSummaryInfo&gt; { private IOwnershipSummaryInfoEditFormFactory _fact; protected override ITypeEditorFormFactoryBase TypeEditorFormFactory { get { if (_fact == null) _fact = TypeEditorsDispatcher.Container.Resolve&lt;IOwnershipSummaryInfoEditFormFactory&gt;(); return _fact; } }  }</v>
+      </c>
+      <c r="F19" t="str">
+        <f t="shared" si="4"/>
+        <v>OwnershipSummaryInfoEditFormFactoryBasic</v>
+      </c>
+      <c r="G19" t="str">
+        <f t="shared" si="5"/>
+        <v>public class OwnershipSummaryInfoEditFormFactoryBasic : IOwnershipSummaryInfoEditFormFactory { public System.Windows.Forms.Form SpawnInstance() { return new DummyForm&lt;OwnershipSummaryInfo &gt;(); } }</v>
+      </c>
+      <c r="H19" t="str">
+        <f t="shared" si="6"/>
+        <v>cont.RegisterInstance&lt;IOwnershipSummaryInfoEditFormFactory&gt;(new OwnershipSummaryInfoEditFormFactoryBasic(), new ContainerControlledLifetimeManager());</v>
+      </c>
+      <c r="I19" t="str">
+        <f t="shared" si="7"/>
+        <v>[System.ComponentModel.Editor(typeof(BGU.DRPL.SignificantOwnership.Core.TypeEditors.OwnershipSummaryInfo_Editor), typeof(System.Drawing.Design.UITypeEditor))]</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>13</v>
+      </c>
+      <c r="B20" t="str">
+        <f t="shared" si="0"/>
+        <v>IOwnershipVotesInfoEditFormFactory</v>
+      </c>
+      <c r="C20" t="str">
+        <f t="shared" si="1"/>
+        <v>public interface IOwnershipVotesInfoEditFormFactory : ITypeEditorFormFactoryBase { }</v>
+      </c>
+      <c r="D20" t="str">
+        <f t="shared" si="2"/>
+        <v>OwnershipVotesInfo_Editor</v>
+      </c>
+      <c r="E20" t="str">
+        <f t="shared" si="3"/>
+        <v>public class OwnershipVotesInfo_Editor : GenericTypeEditor&lt;OwnershipVotesInfo&gt; { private IOwnershipVotesInfoEditFormFactory _fact; protected override ITypeEditorFormFactoryBase TypeEditorFormFactory { get { if (_fact == null) _fact = TypeEditorsDispatcher.Container.Resolve&lt;IOwnershipVotesInfoEditFormFactory&gt;(); return _fact; } }  }</v>
+      </c>
+      <c r="F20" t="str">
+        <f t="shared" si="4"/>
+        <v>OwnershipVotesInfoEditFormFactoryBasic</v>
+      </c>
+      <c r="G20" t="str">
+        <f t="shared" si="5"/>
+        <v>public class OwnershipVotesInfoEditFormFactoryBasic : IOwnershipVotesInfoEditFormFactory { public System.Windows.Forms.Form SpawnInstance() { return new DummyForm&lt;OwnershipVotesInfo &gt;(); } }</v>
+      </c>
+      <c r="H20" t="str">
+        <f t="shared" si="6"/>
+        <v>cont.RegisterInstance&lt;IOwnershipVotesInfoEditFormFactory&gt;(new OwnershipVotesInfoEditFormFactoryBasic(), new ContainerControlledLifetimeManager());</v>
+      </c>
+      <c r="I20" t="str">
+        <f t="shared" si="7"/>
+        <v>[System.ComponentModel.Editor(typeof(BGU.DRPL.SignificantOwnership.Core.TypeEditors.OwnershipVotesInfo_Editor), typeof(System.Drawing.Design.UITypeEditor))]</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>47</v>
+      </c>
+      <c r="B21" t="str">
+        <f t="shared" si="0"/>
+        <v>IPersonsAssociationEditFormFactory</v>
+      </c>
+      <c r="C21" t="str">
+        <f t="shared" si="1"/>
+        <v>public interface IPersonsAssociationEditFormFactory : ITypeEditorFormFactoryBase { }</v>
+      </c>
+      <c r="D21" t="str">
+        <f t="shared" si="2"/>
+        <v>PersonsAssociation_Editor</v>
+      </c>
+      <c r="E21" t="str">
+        <f t="shared" si="3"/>
+        <v>public class PersonsAssociation_Editor : GenericTypeEditor&lt;PersonsAssociation&gt; { private IPersonsAssociationEditFormFactory _fact; protected override ITypeEditorFormFactoryBase TypeEditorFormFactory { get { if (_fact == null) _fact = TypeEditorsDispatcher.Container.Resolve&lt;IPersonsAssociationEditFormFactory&gt;(); return _fact; } }  }</v>
+      </c>
+      <c r="F21" t="str">
+        <f t="shared" si="4"/>
+        <v>PersonsAssociationEditFormFactoryBasic</v>
+      </c>
+      <c r="G21" t="str">
+        <f t="shared" si="5"/>
+        <v>public class PersonsAssociationEditFormFactoryBasic : IPersonsAssociationEditFormFactory { public System.Windows.Forms.Form SpawnInstance() { return new DummyForm&lt;PersonsAssociation &gt;(); } }</v>
+      </c>
+      <c r="H21" t="str">
+        <f t="shared" si="6"/>
+        <v>cont.RegisterInstance&lt;IPersonsAssociationEditFormFactory&gt;(new PersonsAssociationEditFormFactoryBasic(), new ContainerControlledLifetimeManager());</v>
+      </c>
+      <c r="I21" t="str">
+        <f t="shared" si="7"/>
+        <v>[System.ComponentModel.Editor(typeof(BGU.DRPL.SignificantOwnership.Core.TypeEditors.PersonsAssociation_Editor), typeof(System.Drawing.Design.UITypeEditor))]</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>48</v>
+      </c>
+      <c r="B22" t="str">
+        <f t="shared" si="0"/>
+        <v>IPhoneInfoEditFormFactory</v>
+      </c>
+      <c r="C22" t="str">
+        <f t="shared" si="1"/>
+        <v>public interface IPhoneInfoEditFormFactory : ITypeEditorFormFactoryBase { }</v>
+      </c>
+      <c r="D22" t="str">
+        <f t="shared" si="2"/>
+        <v>PhoneInfo_Editor</v>
+      </c>
+      <c r="E22" t="str">
+        <f t="shared" si="3"/>
+        <v>public class PhoneInfo_Editor : GenericTypeEditor&lt;PhoneInfo&gt; { private IPhoneInfoEditFormFactory _fact; protected override ITypeEditorFormFactoryBase TypeEditorFormFactory { get { if (_fact == null) _fact = TypeEditorsDispatcher.Container.Resolve&lt;IPhoneInfoEditFormFactory&gt;(); return _fact; } }  }</v>
+      </c>
+      <c r="F22" t="str">
+        <f t="shared" si="4"/>
+        <v>PhoneInfoEditFormFactoryBasic</v>
+      </c>
+      <c r="G22" t="str">
+        <f t="shared" si="5"/>
+        <v>public class PhoneInfoEditFormFactoryBasic : IPhoneInfoEditFormFactory { public System.Windows.Forms.Form SpawnInstance() { return new DummyForm&lt;PhoneInfo &gt;(); } }</v>
+      </c>
+      <c r="H22" t="str">
+        <f t="shared" si="6"/>
+        <v>cont.RegisterInstance&lt;IPhoneInfoEditFormFactory&gt;(new PhoneInfoEditFormFactoryBasic(), new ContainerControlledLifetimeManager());</v>
+      </c>
+      <c r="I22" t="str">
+        <f t="shared" si="7"/>
+        <v>[System.ComponentModel.Editor(typeof(BGU.DRPL.SignificantOwnership.Core.TypeEditors.PhoneInfo_Editor), typeof(System.Drawing.Design.UITypeEditor))]</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>14</v>
+      </c>
+      <c r="B23" t="str">
+        <f t="shared" si="0"/>
+        <v>IPhysicalPersonShareInfoEditFormFactory</v>
+      </c>
+      <c r="C23" t="str">
+        <f t="shared" si="1"/>
+        <v>public interface IPhysicalPersonShareInfoEditFormFactory : ITypeEditorFormFactoryBase { }</v>
+      </c>
+      <c r="D23" t="str">
+        <f t="shared" si="2"/>
+        <v>PhysicalPersonShareInfo_Editor</v>
+      </c>
+      <c r="E23" t="str">
+        <f t="shared" si="3"/>
+        <v>public class PhysicalPersonShareInfo_Editor : GenericTypeEditor&lt;PhysicalPersonShareInfo&gt; { private IPhysicalPersonShareInfoEditFormFactory _fact; protected override ITypeEditorFormFactoryBase TypeEditorFormFactory { get { if (_fact == null) _fact = TypeEditorsDispatcher.Container.Resolve&lt;IPhysicalPersonShareInfoEditFormFactory&gt;(); return _fact; } }  }</v>
+      </c>
+      <c r="F23" t="str">
+        <f t="shared" si="4"/>
+        <v>PhysicalPersonShareInfoEditFormFactoryBasic</v>
+      </c>
+      <c r="G23" t="str">
+        <f t="shared" si="5"/>
+        <v>public class PhysicalPersonShareInfoEditFormFactoryBasic : IPhysicalPersonShareInfoEditFormFactory { public System.Windows.Forms.Form SpawnInstance() { return new DummyForm&lt;PhysicalPersonShareInfo &gt;(); } }</v>
+      </c>
+      <c r="H23" t="str">
+        <f t="shared" si="6"/>
+        <v>cont.RegisterInstance&lt;IPhysicalPersonShareInfoEditFormFactory&gt;(new PhysicalPersonShareInfoEditFormFactoryBasic(), new ContainerControlledLifetimeManager());</v>
+      </c>
+      <c r="I23" t="str">
+        <f t="shared" si="7"/>
+        <v>[System.ComponentModel.Editor(typeof(BGU.DRPL.SignificantOwnership.Core.TypeEditors.PhysicalPersonShareInfo_Editor), typeof(System.Drawing.Design.UITypeEditor))]</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>49</v>
+      </c>
+      <c r="B24" t="str">
+        <f t="shared" si="0"/>
+        <v>IPurchasedVoteInfoEditFormFactory</v>
+      </c>
+      <c r="C24" t="str">
+        <f t="shared" si="1"/>
+        <v>public interface IPurchasedVoteInfoEditFormFactory : ITypeEditorFormFactoryBase { }</v>
+      </c>
+      <c r="D24" t="str">
+        <f t="shared" si="2"/>
+        <v>PurchasedVoteInfo_Editor</v>
+      </c>
+      <c r="E24" t="str">
+        <f t="shared" si="3"/>
+        <v>public class PurchasedVoteInfo_Editor : GenericTypeEditor&lt;PurchasedVoteInfo&gt; { private IPurchasedVoteInfoEditFormFactory _fact; protected override ITypeEditorFormFactoryBase TypeEditorFormFactory { get { if (_fact == null) _fact = TypeEditorsDispatcher.Container.Resolve&lt;IPurchasedVoteInfoEditFormFactory&gt;(); return _fact; } }  }</v>
+      </c>
+      <c r="F24" t="str">
+        <f t="shared" si="4"/>
+        <v>PurchasedVoteInfoEditFormFactoryBasic</v>
+      </c>
+      <c r="G24" t="str">
+        <f t="shared" si="5"/>
+        <v>public class PurchasedVoteInfoEditFormFactoryBasic : IPurchasedVoteInfoEditFormFactory { public System.Windows.Forms.Form SpawnInstance() { return new DummyForm&lt;PurchasedVoteInfo &gt;(); } }</v>
+      </c>
+      <c r="H24" t="str">
+        <f t="shared" si="6"/>
+        <v>cont.RegisterInstance&lt;IPurchasedVoteInfoEditFormFactory&gt;(new PurchasedVoteInfoEditFormFactoryBasic(), new ContainerControlledLifetimeManager());</v>
+      </c>
+      <c r="I24" t="str">
+        <f t="shared" si="7"/>
+        <v>[System.ComponentModel.Editor(typeof(BGU.DRPL.SignificantOwnership.Core.TypeEditors.PurchasedVoteInfo_Editor), typeof(System.Drawing.Design.UITypeEditor))]</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>15</v>
+      </c>
+      <c r="B25" t="str">
+        <f t="shared" si="0"/>
+        <v>ISignatoryInfoEditFormFactory</v>
+      </c>
+      <c r="C25" t="str">
+        <f t="shared" si="1"/>
+        <v>public interface ISignatoryInfoEditFormFactory : ITypeEditorFormFactoryBase { }</v>
+      </c>
+      <c r="D25" t="str">
+        <f t="shared" si="2"/>
+        <v>SignatoryInfo_Editor</v>
+      </c>
+      <c r="E25" t="str">
+        <f t="shared" si="3"/>
+        <v>public class SignatoryInfo_Editor : GenericTypeEditor&lt;SignatoryInfo&gt; { private ISignatoryInfoEditFormFactory _fact; protected override ITypeEditorFormFactoryBase TypeEditorFormFactory { get { if (_fact == null) _fact = TypeEditorsDispatcher.Container.Resolve&lt;ISignatoryInfoEditFormFactory&gt;(); return _fact; } }  }</v>
+      </c>
+      <c r="F25" t="str">
+        <f t="shared" si="4"/>
+        <v>SignatoryInfoEditFormFactoryBasic</v>
+      </c>
+      <c r="G25" t="str">
+        <f t="shared" si="5"/>
+        <v>public class SignatoryInfoEditFormFactoryBasic : ISignatoryInfoEditFormFactory { public System.Windows.Forms.Form SpawnInstance() { return new DummyForm&lt;SignatoryInfo &gt;(); } }</v>
+      </c>
+      <c r="H25" t="str">
+        <f t="shared" si="6"/>
+        <v>cont.RegisterInstance&lt;ISignatoryInfoEditFormFactory&gt;(new SignatoryInfoEditFormFactoryBasic(), new ContainerControlledLifetimeManager());</v>
+      </c>
+      <c r="I25" t="str">
+        <f t="shared" si="7"/>
+        <v>[System.ComponentModel.Editor(typeof(BGU.DRPL.SignificantOwnership.Core.TypeEditors.SignatoryInfo_Editor), typeof(System.Drawing.Design.UITypeEditor))]</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>16</v>
+      </c>
+      <c r="B26" t="str">
+        <f t="shared" si="0"/>
+        <v>ITotalOwnershipDetailsInfoEditFormFactory</v>
+      </c>
+      <c r="C26" t="str">
+        <f t="shared" si="1"/>
+        <v>public interface ITotalOwnershipDetailsInfoEditFormFactory : ITypeEditorFormFactoryBase { }</v>
+      </c>
+      <c r="D26" t="str">
+        <f t="shared" si="2"/>
+        <v>TotalOwnershipDetailsInfo_Editor</v>
+      </c>
+      <c r="E26" t="str">
+        <f t="shared" si="3"/>
+        <v>public class TotalOwnershipDetailsInfo_Editor : GenericTypeEditor&lt;TotalOwnershipDetailsInfo&gt; { private ITotalOwnershipDetailsInfoEditFormFactory _fact; protected override ITypeEditorFormFactoryBase TypeEditorFormFactory { get { if (_fact == null) _fact = TypeEditorsDispatcher.Container.Resolve&lt;ITotalOwnershipDetailsInfoEditFormFactory&gt;(); return _fact; } }  }</v>
+      </c>
+      <c r="F26" t="str">
+        <f t="shared" si="4"/>
+        <v>TotalOwnershipDetailsInfoEditFormFactoryBasic</v>
+      </c>
+      <c r="G26" t="str">
+        <f t="shared" si="5"/>
+        <v>public class TotalOwnershipDetailsInfoEditFormFactoryBasic : ITotalOwnershipDetailsInfoEditFormFactory { public System.Windows.Forms.Form SpawnInstance() { return new DummyForm&lt;TotalOwnershipDetailsInfo &gt;(); } }</v>
+      </c>
+      <c r="H26" t="str">
+        <f t="shared" si="6"/>
+        <v>cont.RegisterInstance&lt;ITotalOwnershipDetailsInfoEditFormFactory&gt;(new TotalOwnershipDetailsInfoEditFormFactoryBasic(), new ContainerControlledLifetimeManager());</v>
+      </c>
+      <c r="I26" t="str">
+        <f t="shared" si="7"/>
+        <v>[System.ComponentModel.Editor(typeof(BGU.DRPL.SignificantOwnership.Core.TypeEditors.TotalOwnershipDetailsInfo_Editor), typeof(System.Drawing.Design.UITypeEditor))]</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>17</v>
+      </c>
+      <c r="B27" t="str">
+        <f t="shared" si="0"/>
+        <v>IBankInfoEditFormFactory</v>
+      </c>
+      <c r="C27" t="str">
+        <f t="shared" si="1"/>
+        <v>public interface IBankInfoEditFormFactory : ITypeEditorFormFactoryBase { }</v>
+      </c>
+      <c r="D27" t="str">
+        <f t="shared" si="2"/>
+        <v>BankInfo_Editor</v>
+      </c>
+      <c r="E27" t="str">
+        <f t="shared" si="3"/>
+        <v>public class BankInfo_Editor : GenericTypeEditor&lt;BankInfo&gt; { private IBankInfoEditFormFactory _fact; protected override ITypeEditorFormFactoryBase TypeEditorFormFactory { get { if (_fact == null) _fact = TypeEditorsDispatcher.Container.Resolve&lt;IBankInfoEditFormFactory&gt;(); return _fact; } }  }</v>
+      </c>
+      <c r="F27" t="str">
+        <f t="shared" si="4"/>
+        <v>BankInfoEditFormFactoryBasic</v>
+      </c>
+      <c r="G27" t="str">
+        <f t="shared" si="5"/>
+        <v>public class BankInfoEditFormFactoryBasic : IBankInfoEditFormFactory { public System.Windows.Forms.Form SpawnInstance() { return new DummyForm&lt;BankInfo &gt;(); } }</v>
+      </c>
+      <c r="H27" t="str">
+        <f t="shared" si="6"/>
+        <v>cont.RegisterInstance&lt;IBankInfoEditFormFactory&gt;(new BankInfoEditFormFactoryBasic(), new ContainerControlledLifetimeManager());</v>
+      </c>
+      <c r="I27" t="str">
+        <f t="shared" si="7"/>
+        <v>[System.ComponentModel.Editor(typeof(BGU.DRPL.SignificantOwnership.Core.TypeEditors.BankInfo_Editor), typeof(System.Drawing.Design.UITypeEditor))]</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>18</v>
+      </c>
+      <c r="B28" t="str">
+        <f t="shared" si="0"/>
+        <v>ICountryInfoEditFormFactory</v>
+      </c>
+      <c r="C28" t="str">
+        <f t="shared" si="1"/>
+        <v>public interface ICountryInfoEditFormFactory : ITypeEditorFormFactoryBase { }</v>
+      </c>
+      <c r="D28" t="str">
+        <f t="shared" si="2"/>
+        <v>CountryInfo_Editor</v>
+      </c>
+      <c r="E28" t="str">
+        <f t="shared" si="3"/>
+        <v>public class CountryInfo_Editor : GenericTypeEditor&lt;CountryInfo&gt; { private ICountryInfoEditFormFactory _fact; protected override ITypeEditorFormFactoryBase TypeEditorFormFactory { get { if (_fact == null) _fact = TypeEditorsDispatcher.Container.Resolve&lt;ICountryInfoEditFormFactory&gt;(); return _fact; } }  }</v>
+      </c>
+      <c r="F28" t="str">
+        <f t="shared" si="4"/>
+        <v>CountryInfoEditFormFactoryBasic</v>
+      </c>
+      <c r="G28" t="str">
+        <f t="shared" si="5"/>
+        <v>public class CountryInfoEditFormFactoryBasic : ICountryInfoEditFormFactory { public System.Windows.Forms.Form SpawnInstance() { return new DummyForm&lt;CountryInfo &gt;(); } }</v>
+      </c>
+      <c r="H28" t="str">
+        <f t="shared" si="6"/>
+        <v>cont.RegisterInstance&lt;ICountryInfoEditFormFactory&gt;(new CountryInfoEditFormFactoryBasic(), new ContainerControlledLifetimeManager());</v>
+      </c>
+      <c r="I28" t="str">
+        <f t="shared" si="7"/>
+        <v>[System.ComponentModel.Editor(typeof(BGU.DRPL.SignificantOwnership.Core.TypeEditors.CountryInfo_Editor), typeof(System.Drawing.Design.UITypeEditor))]</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>19</v>
+      </c>
+      <c r="B29" t="str">
+        <f t="shared" si="0"/>
+        <v>ILegalPersonInfoEditFormFactory</v>
+      </c>
+      <c r="C29" t="str">
+        <f t="shared" si="1"/>
+        <v>public interface ILegalPersonInfoEditFormFactory : ITypeEditorFormFactoryBase { }</v>
+      </c>
+      <c r="D29" t="str">
+        <f t="shared" si="2"/>
+        <v>LegalPersonInfo_Editor</v>
+      </c>
+      <c r="E29" t="str">
+        <f t="shared" si="3"/>
+        <v>public class LegalPersonInfo_Editor : GenericTypeEditor&lt;LegalPersonInfo&gt; { private ILegalPersonInfoEditFormFactory _fact; protected override ITypeEditorFormFactoryBase TypeEditorFormFactory { get { if (_fact == null) _fact = TypeEditorsDispatcher.Container.Resolve&lt;ILegalPersonInfoEditFormFactory&gt;(); return _fact; } }  }</v>
+      </c>
+      <c r="F29" t="str">
+        <f t="shared" si="4"/>
+        <v>LegalPersonInfoEditFormFactoryBasic</v>
+      </c>
+      <c r="G29" t="str">
+        <f t="shared" si="5"/>
+        <v>public class LegalPersonInfoEditFormFactoryBasic : ILegalPersonInfoEditFormFactory { public System.Windows.Forms.Form SpawnInstance() { return new DummyForm&lt;LegalPersonInfo &gt;(); } }</v>
+      </c>
+      <c r="H29" t="str">
+        <f t="shared" si="6"/>
+        <v>cont.RegisterInstance&lt;ILegalPersonInfoEditFormFactory&gt;(new LegalPersonInfoEditFormFactoryBasic(), new ContainerControlledLifetimeManager());</v>
+      </c>
+      <c r="I29" t="str">
+        <f t="shared" si="7"/>
+        <v>[System.ComponentModel.Editor(typeof(BGU.DRPL.SignificantOwnership.Core.TypeEditors.LegalPersonInfo_Editor), typeof(System.Drawing.Design.UITypeEditor))]</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>20</v>
+      </c>
+      <c r="B30" t="str">
+        <f t="shared" si="0"/>
+        <v>ILocationInfoEditFormFactory</v>
+      </c>
+      <c r="C30" t="str">
+        <f t="shared" si="1"/>
+        <v>public interface ILocationInfoEditFormFactory : ITypeEditorFormFactoryBase { }</v>
+      </c>
+      <c r="D30" t="str">
+        <f t="shared" si="2"/>
+        <v>LocationInfo_Editor</v>
+      </c>
+      <c r="E30" t="str">
+        <f t="shared" si="3"/>
+        <v>public class LocationInfo_Editor : GenericTypeEditor&lt;LocationInfo&gt; { private ILocationInfoEditFormFactory _fact; protected override ITypeEditorFormFactoryBase TypeEditorFormFactory { get { if (_fact == null) _fact = TypeEditorsDispatcher.Container.Resolve&lt;ILocationInfoEditFormFactory&gt;(); return _fact; } }  }</v>
+      </c>
+      <c r="F30" t="str">
+        <f t="shared" si="4"/>
+        <v>LocationInfoEditFormFactoryBasic</v>
+      </c>
+      <c r="G30" t="str">
+        <f t="shared" si="5"/>
+        <v>public class LocationInfoEditFormFactoryBasic : ILocationInfoEditFormFactory { public System.Windows.Forms.Form SpawnInstance() { return new DummyForm&lt;LocationInfo &gt;(); } }</v>
+      </c>
+      <c r="H30" t="str">
+        <f t="shared" si="6"/>
+        <v>cont.RegisterInstance&lt;ILocationInfoEditFormFactory&gt;(new LocationInfoEditFormFactoryBasic(), new ContainerControlledLifetimeManager());</v>
+      </c>
+      <c r="I30" t="str">
+        <f t="shared" si="7"/>
+        <v>[System.ComponentModel.Editor(typeof(BGU.DRPL.SignificantOwnership.Core.TypeEditors.LocationInfo_Editor), typeof(System.Drawing.Design.UITypeEditor))]</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>22</v>
+      </c>
+      <c r="B31" t="str">
+        <f t="shared" si="0"/>
+        <v>IPhysicalPersonInfoEditFormFactory</v>
+      </c>
+      <c r="C31" t="str">
+        <f t="shared" si="1"/>
+        <v>public interface IPhysicalPersonInfoEditFormFactory : ITypeEditorFormFactoryBase { }</v>
+      </c>
+      <c r="D31" t="str">
+        <f t="shared" si="2"/>
+        <v>PhysicalPersonInfo_Editor</v>
+      </c>
+      <c r="E31" t="str">
+        <f t="shared" si="3"/>
+        <v>public class PhysicalPersonInfo_Editor : GenericTypeEditor&lt;PhysicalPersonInfo&gt; { private IPhysicalPersonInfoEditFormFactory _fact; protected override ITypeEditorFormFactoryBase TypeEditorFormFactory { get { if (_fact == null) _fact = TypeEditorsDispatcher.Container.Resolve&lt;IPhysicalPersonInfoEditFormFactory&gt;(); return _fact; } }  }</v>
+      </c>
+      <c r="F31" t="str">
+        <f t="shared" si="4"/>
+        <v>PhysicalPersonInfoEditFormFactoryBasic</v>
+      </c>
+      <c r="G31" t="str">
+        <f t="shared" si="5"/>
+        <v>public class PhysicalPersonInfoEditFormFactoryBasic : IPhysicalPersonInfoEditFormFactory { public System.Windows.Forms.Form SpawnInstance() { return new DummyForm&lt;PhysicalPersonInfo &gt;(); } }</v>
+      </c>
+      <c r="H31" t="str">
+        <f t="shared" si="6"/>
+        <v>cont.RegisterInstance&lt;IPhysicalPersonInfoEditFormFactory&gt;(new PhysicalPersonInfoEditFormFactoryBasic(), new ContainerControlledLifetimeManager());</v>
+      </c>
+      <c r="I31" t="str">
+        <f t="shared" si="7"/>
+        <v>[System.ComponentModel.Editor(typeof(BGU.DRPL.SignificantOwnership.Core.TypeEditors.PhysicalPersonInfo_Editor), typeof(System.Drawing.Design.UITypeEditor))]</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>23</v>
+      </c>
+      <c r="B32" t="str">
+        <f t="shared" si="0"/>
+        <v>IRegistrarAuthorityEditFormFactory</v>
+      </c>
+      <c r="C32" t="str">
+        <f t="shared" si="1"/>
+        <v>public interface IRegistrarAuthorityEditFormFactory : ITypeEditorFormFactoryBase { }</v>
+      </c>
+      <c r="D32" t="str">
+        <f t="shared" si="2"/>
+        <v>RegistrarAuthority_Editor</v>
+      </c>
+      <c r="E32" t="str">
+        <f t="shared" si="3"/>
+        <v>public class RegistrarAuthority_Editor : GenericTypeEditor&lt;RegistrarAuthority&gt; { private IRegistrarAuthorityEditFormFactory _fact; protected override ITypeEditorFormFactoryBase TypeEditorFormFactory { get { if (_fact == null) _fact = TypeEditorsDispatcher.Container.Resolve&lt;IRegistrarAuthorityEditFormFactory&gt;(); return _fact; } }  }</v>
+      </c>
+      <c r="F32" t="str">
+        <f t="shared" si="4"/>
+        <v>RegistrarAuthorityEditFormFactoryBasic</v>
+      </c>
+      <c r="G32" t="str">
+        <f t="shared" si="5"/>
+        <v>public class RegistrarAuthorityEditFormFactoryBasic : IRegistrarAuthorityEditFormFactory { public System.Windows.Forms.Form SpawnInstance() { return new DummyForm&lt;RegistrarAuthority &gt;(); } }</v>
+      </c>
+      <c r="H32" t="str">
+        <f t="shared" si="6"/>
+        <v>cont.RegisterInstance&lt;IRegistrarAuthorityEditFormFactory&gt;(new RegistrarAuthorityEditFormFactoryBasic(), new ContainerControlledLifetimeManager());</v>
+      </c>
+      <c r="I32" t="str">
+        <f t="shared" si="7"/>
+        <v>[System.ComponentModel.Editor(typeof(BGU.DRPL.SignificantOwnership.Core.TypeEditors.RegistrarAuthority_Editor), typeof(System.Drawing.Design.UITypeEditor))]</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
+* BGU-14 RegNLic: АНКЕТА фізичної особи (Додаток 4) - done, incl. DisplayName's and Description's
</commit_message>
<xml_diff>
--- a/BGU.DRPL.SignificantOwnership/Codegen/BGU_xsd_outil16.xlsx
+++ b/BGU.DRPL.SignificantOwnership/Codegen/BGU_xsd_outil16.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="69">
   <si>
     <t>ClassName</t>
   </si>
@@ -176,6 +176,63 @@
   </si>
   <si>
     <t>PurchasedVoteInfo</t>
+  </si>
+  <si>
+    <t>BreachOfLawRecordInfo</t>
+  </si>
+  <si>
+    <t>EducationRecordInfo</t>
+  </si>
+  <si>
+    <t>EmploymentRecordInfo</t>
+  </si>
+  <si>
+    <t>FinancialGuaranteeInfo</t>
+  </si>
+  <si>
+    <t>IncomeOriginInfo</t>
+  </si>
+  <si>
+    <t>IndebtnessInfo</t>
+  </si>
+  <si>
+    <t>IndebtnessInfoBase</t>
+  </si>
+  <si>
+    <t>LiquidatedEntityOwnershipInfo</t>
+  </si>
+  <si>
+    <t>LoanInfo</t>
+  </si>
+  <si>
+    <t>PaymentDeadlineInfo</t>
+  </si>
+  <si>
+    <t>PaymentModeInfo</t>
+  </si>
+  <si>
+    <t>ProfessionLicenseInfo</t>
+  </si>
+  <si>
+    <t>SharesAcquisitionInfo</t>
+  </si>
+  <si>
+    <t>BankAccountInfo</t>
+  </si>
+  <si>
+    <t>ProfessionLicensingBodyInfo</t>
+  </si>
+  <si>
+    <t>PublicationInfo</t>
+  </si>
+  <si>
+    <t>PublishingHouseInfo</t>
+  </si>
+  <si>
+    <t>UniversityOrCollegeInfo</t>
+  </si>
+  <si>
+    <t>FinancialOversightAuthorityInfo</t>
   </si>
 </sst>
 </file>
@@ -990,10 +1047,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I32"/>
+  <dimension ref="A1:I51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="I32" sqref="I32"/>
+    <sheetView tabSelected="1" topLeftCell="A24" workbookViewId="0">
+      <selection activeCell="G51" sqref="G51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2182,6 +2239,709 @@
         <v>[System.ComponentModel.Editor(typeof(BGU.DRPL.SignificantOwnership.Core.TypeEditors.RegistrarAuthority_Editor), typeof(System.Drawing.Design.UITypeEditor))]</v>
       </c>
     </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>50</v>
+      </c>
+      <c r="B33" t="str">
+        <f t="shared" ref="B33:B50" si="8">"I"&amp; TRIM(A33) &amp; "EditFormFactory"</f>
+        <v>IBreachOfLawRecordInfoEditFormFactory</v>
+      </c>
+      <c r="C33" t="str">
+        <f t="shared" ref="C33:C50" si="9">"public interface I"&amp; TRIM(A33) &amp; "EditFormFactory : ITypeEditorFormFactoryBase { }"</f>
+        <v>public interface IBreachOfLawRecordInfoEditFormFactory : ITypeEditorFormFactoryBase { }</v>
+      </c>
+      <c r="D33" t="str">
+        <f t="shared" ref="D33:D50" si="10">A33&amp; "_Editor"</f>
+        <v>BreachOfLawRecordInfo_Editor</v>
+      </c>
+      <c r="E33" t="str">
+        <f t="shared" ref="E33:E50" si="11">"public class " &amp; D33 &amp; " : GenericTypeEditor&lt;"&amp;A33&amp;"&gt; { private " &amp; B33 &amp; " _fact; protected override ITypeEditorFormFactoryBase TypeEditorFormFactory { get { if (_fact == null) _fact = TypeEditorsDispatcher.Container.Resolve&lt;" &amp;B33 &amp; "&gt;(); return _fact; } }  }"</f>
+        <v>public class BreachOfLawRecordInfo_Editor : GenericTypeEditor&lt;BreachOfLawRecordInfo&gt; { private IBreachOfLawRecordInfoEditFormFactory _fact; protected override ITypeEditorFormFactoryBase TypeEditorFormFactory { get { if (_fact == null) _fact = TypeEditorsDispatcher.Container.Resolve&lt;IBreachOfLawRecordInfoEditFormFactory&gt;(); return _fact; } }  }</v>
+      </c>
+      <c r="F33" t="str">
+        <f t="shared" ref="F33:F50" si="12">A33&amp; "EditFormFactoryBasic"</f>
+        <v>BreachOfLawRecordInfoEditFormFactoryBasic</v>
+      </c>
+      <c r="G33" t="str">
+        <f t="shared" ref="G33:G50" si="13">"public class " &amp;F33&amp; " : " &amp; B33 &amp; " { public System.Windows.Forms.Form SpawnInstance() { return new DummyForm&lt;" &amp;A33&amp; " &gt;(); } }"</f>
+        <v>public class BreachOfLawRecordInfoEditFormFactoryBasic : IBreachOfLawRecordInfoEditFormFactory { public System.Windows.Forms.Form SpawnInstance() { return new DummyForm&lt;BreachOfLawRecordInfo &gt;(); } }</v>
+      </c>
+      <c r="H33" t="str">
+        <f t="shared" ref="H33:H50" si="14">"cont.RegisterInstance&lt;" &amp; B33 &amp; "&gt;(new " &amp; F33 &amp; "(), new ContainerControlledLifetimeManager());"</f>
+        <v>cont.RegisterInstance&lt;IBreachOfLawRecordInfoEditFormFactory&gt;(new BreachOfLawRecordInfoEditFormFactoryBasic(), new ContainerControlledLifetimeManager());</v>
+      </c>
+      <c r="I33" t="str">
+        <f t="shared" ref="I33:I50" si="15">"[System.ComponentModel.Editor(typeof(BGU.DRPL.SignificantOwnership.Core.TypeEditors." &amp;D33 &amp; "), typeof(System.Drawing.Design.UITypeEditor))]"</f>
+        <v>[System.ComponentModel.Editor(typeof(BGU.DRPL.SignificantOwnership.Core.TypeEditors.BreachOfLawRecordInfo_Editor), typeof(System.Drawing.Design.UITypeEditor))]</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>51</v>
+      </c>
+      <c r="B34" t="str">
+        <f t="shared" si="8"/>
+        <v>IEducationRecordInfoEditFormFactory</v>
+      </c>
+      <c r="C34" t="str">
+        <f t="shared" si="9"/>
+        <v>public interface IEducationRecordInfoEditFormFactory : ITypeEditorFormFactoryBase { }</v>
+      </c>
+      <c r="D34" t="str">
+        <f t="shared" si="10"/>
+        <v>EducationRecordInfo_Editor</v>
+      </c>
+      <c r="E34" t="str">
+        <f t="shared" si="11"/>
+        <v>public class EducationRecordInfo_Editor : GenericTypeEditor&lt;EducationRecordInfo&gt; { private IEducationRecordInfoEditFormFactory _fact; protected override ITypeEditorFormFactoryBase TypeEditorFormFactory { get { if (_fact == null) _fact = TypeEditorsDispatcher.Container.Resolve&lt;IEducationRecordInfoEditFormFactory&gt;(); return _fact; } }  }</v>
+      </c>
+      <c r="F34" t="str">
+        <f t="shared" si="12"/>
+        <v>EducationRecordInfoEditFormFactoryBasic</v>
+      </c>
+      <c r="G34" t="str">
+        <f t="shared" si="13"/>
+        <v>public class EducationRecordInfoEditFormFactoryBasic : IEducationRecordInfoEditFormFactory { public System.Windows.Forms.Form SpawnInstance() { return new DummyForm&lt;EducationRecordInfo &gt;(); } }</v>
+      </c>
+      <c r="H34" t="str">
+        <f t="shared" si="14"/>
+        <v>cont.RegisterInstance&lt;IEducationRecordInfoEditFormFactory&gt;(new EducationRecordInfoEditFormFactoryBasic(), new ContainerControlledLifetimeManager());</v>
+      </c>
+      <c r="I34" t="str">
+        <f t="shared" si="15"/>
+        <v>[System.ComponentModel.Editor(typeof(BGU.DRPL.SignificantOwnership.Core.TypeEditors.EducationRecordInfo_Editor), typeof(System.Drawing.Design.UITypeEditor))]</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>52</v>
+      </c>
+      <c r="B35" t="str">
+        <f t="shared" si="8"/>
+        <v>IEmploymentRecordInfoEditFormFactory</v>
+      </c>
+      <c r="C35" t="str">
+        <f t="shared" si="9"/>
+        <v>public interface IEmploymentRecordInfoEditFormFactory : ITypeEditorFormFactoryBase { }</v>
+      </c>
+      <c r="D35" t="str">
+        <f t="shared" si="10"/>
+        <v>EmploymentRecordInfo_Editor</v>
+      </c>
+      <c r="E35" t="str">
+        <f t="shared" si="11"/>
+        <v>public class EmploymentRecordInfo_Editor : GenericTypeEditor&lt;EmploymentRecordInfo&gt; { private IEmploymentRecordInfoEditFormFactory _fact; protected override ITypeEditorFormFactoryBase TypeEditorFormFactory { get { if (_fact == null) _fact = TypeEditorsDispatcher.Container.Resolve&lt;IEmploymentRecordInfoEditFormFactory&gt;(); return _fact; } }  }</v>
+      </c>
+      <c r="F35" t="str">
+        <f t="shared" si="12"/>
+        <v>EmploymentRecordInfoEditFormFactoryBasic</v>
+      </c>
+      <c r="G35" t="str">
+        <f t="shared" si="13"/>
+        <v>public class EmploymentRecordInfoEditFormFactoryBasic : IEmploymentRecordInfoEditFormFactory { public System.Windows.Forms.Form SpawnInstance() { return new DummyForm&lt;EmploymentRecordInfo &gt;(); } }</v>
+      </c>
+      <c r="H35" t="str">
+        <f t="shared" si="14"/>
+        <v>cont.RegisterInstance&lt;IEmploymentRecordInfoEditFormFactory&gt;(new EmploymentRecordInfoEditFormFactoryBasic(), new ContainerControlledLifetimeManager());</v>
+      </c>
+      <c r="I35" t="str">
+        <f t="shared" si="15"/>
+        <v>[System.ComponentModel.Editor(typeof(BGU.DRPL.SignificantOwnership.Core.TypeEditors.EmploymentRecordInfo_Editor), typeof(System.Drawing.Design.UITypeEditor))]</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>53</v>
+      </c>
+      <c r="B36" t="str">
+        <f t="shared" si="8"/>
+        <v>IFinancialGuaranteeInfoEditFormFactory</v>
+      </c>
+      <c r="C36" t="str">
+        <f t="shared" si="9"/>
+        <v>public interface IFinancialGuaranteeInfoEditFormFactory : ITypeEditorFormFactoryBase { }</v>
+      </c>
+      <c r="D36" t="str">
+        <f t="shared" si="10"/>
+        <v>FinancialGuaranteeInfo_Editor</v>
+      </c>
+      <c r="E36" t="str">
+        <f t="shared" si="11"/>
+        <v>public class FinancialGuaranteeInfo_Editor : GenericTypeEditor&lt;FinancialGuaranteeInfo&gt; { private IFinancialGuaranteeInfoEditFormFactory _fact; protected override ITypeEditorFormFactoryBase TypeEditorFormFactory { get { if (_fact == null) _fact = TypeEditorsDispatcher.Container.Resolve&lt;IFinancialGuaranteeInfoEditFormFactory&gt;(); return _fact; } }  }</v>
+      </c>
+      <c r="F36" t="str">
+        <f t="shared" si="12"/>
+        <v>FinancialGuaranteeInfoEditFormFactoryBasic</v>
+      </c>
+      <c r="G36" t="str">
+        <f t="shared" si="13"/>
+        <v>public class FinancialGuaranteeInfoEditFormFactoryBasic : IFinancialGuaranteeInfoEditFormFactory { public System.Windows.Forms.Form SpawnInstance() { return new DummyForm&lt;FinancialGuaranteeInfo &gt;(); } }</v>
+      </c>
+      <c r="H36" t="str">
+        <f t="shared" si="14"/>
+        <v>cont.RegisterInstance&lt;IFinancialGuaranteeInfoEditFormFactory&gt;(new FinancialGuaranteeInfoEditFormFactoryBasic(), new ContainerControlledLifetimeManager());</v>
+      </c>
+      <c r="I36" t="str">
+        <f t="shared" si="15"/>
+        <v>[System.ComponentModel.Editor(typeof(BGU.DRPL.SignificantOwnership.Core.TypeEditors.FinancialGuaranteeInfo_Editor), typeof(System.Drawing.Design.UITypeEditor))]</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>54</v>
+      </c>
+      <c r="B37" t="str">
+        <f t="shared" si="8"/>
+        <v>IIncomeOriginInfoEditFormFactory</v>
+      </c>
+      <c r="C37" t="str">
+        <f t="shared" si="9"/>
+        <v>public interface IIncomeOriginInfoEditFormFactory : ITypeEditorFormFactoryBase { }</v>
+      </c>
+      <c r="D37" t="str">
+        <f t="shared" si="10"/>
+        <v>IncomeOriginInfo_Editor</v>
+      </c>
+      <c r="E37" t="str">
+        <f t="shared" si="11"/>
+        <v>public class IncomeOriginInfo_Editor : GenericTypeEditor&lt;IncomeOriginInfo&gt; { private IIncomeOriginInfoEditFormFactory _fact; protected override ITypeEditorFormFactoryBase TypeEditorFormFactory { get { if (_fact == null) _fact = TypeEditorsDispatcher.Container.Resolve&lt;IIncomeOriginInfoEditFormFactory&gt;(); return _fact; } }  }</v>
+      </c>
+      <c r="F37" t="str">
+        <f t="shared" si="12"/>
+        <v>IncomeOriginInfoEditFormFactoryBasic</v>
+      </c>
+      <c r="G37" t="str">
+        <f t="shared" si="13"/>
+        <v>public class IncomeOriginInfoEditFormFactoryBasic : IIncomeOriginInfoEditFormFactory { public System.Windows.Forms.Form SpawnInstance() { return new DummyForm&lt;IncomeOriginInfo &gt;(); } }</v>
+      </c>
+      <c r="H37" t="str">
+        <f t="shared" si="14"/>
+        <v>cont.RegisterInstance&lt;IIncomeOriginInfoEditFormFactory&gt;(new IncomeOriginInfoEditFormFactoryBasic(), new ContainerControlledLifetimeManager());</v>
+      </c>
+      <c r="I37" t="str">
+        <f t="shared" si="15"/>
+        <v>[System.ComponentModel.Editor(typeof(BGU.DRPL.SignificantOwnership.Core.TypeEditors.IncomeOriginInfo_Editor), typeof(System.Drawing.Design.UITypeEditor))]</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>55</v>
+      </c>
+      <c r="B38" t="str">
+        <f t="shared" si="8"/>
+        <v>IIndebtnessInfoEditFormFactory</v>
+      </c>
+      <c r="C38" t="str">
+        <f t="shared" si="9"/>
+        <v>public interface IIndebtnessInfoEditFormFactory : ITypeEditorFormFactoryBase { }</v>
+      </c>
+      <c r="D38" t="str">
+        <f t="shared" si="10"/>
+        <v>IndebtnessInfo_Editor</v>
+      </c>
+      <c r="E38" t="str">
+        <f t="shared" si="11"/>
+        <v>public class IndebtnessInfo_Editor : GenericTypeEditor&lt;IndebtnessInfo&gt; { private IIndebtnessInfoEditFormFactory _fact; protected override ITypeEditorFormFactoryBase TypeEditorFormFactory { get { if (_fact == null) _fact = TypeEditorsDispatcher.Container.Resolve&lt;IIndebtnessInfoEditFormFactory&gt;(); return _fact; } }  }</v>
+      </c>
+      <c r="F38" t="str">
+        <f t="shared" si="12"/>
+        <v>IndebtnessInfoEditFormFactoryBasic</v>
+      </c>
+      <c r="G38" t="str">
+        <f t="shared" si="13"/>
+        <v>public class IndebtnessInfoEditFormFactoryBasic : IIndebtnessInfoEditFormFactory { public System.Windows.Forms.Form SpawnInstance() { return new DummyForm&lt;IndebtnessInfo &gt;(); } }</v>
+      </c>
+      <c r="H38" t="str">
+        <f t="shared" si="14"/>
+        <v>cont.RegisterInstance&lt;IIndebtnessInfoEditFormFactory&gt;(new IndebtnessInfoEditFormFactoryBasic(), new ContainerControlledLifetimeManager());</v>
+      </c>
+      <c r="I38" t="str">
+        <f t="shared" si="15"/>
+        <v>[System.ComponentModel.Editor(typeof(BGU.DRPL.SignificantOwnership.Core.TypeEditors.IndebtnessInfo_Editor), typeof(System.Drawing.Design.UITypeEditor))]</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>56</v>
+      </c>
+      <c r="B39" t="str">
+        <f t="shared" si="8"/>
+        <v>IIndebtnessInfoBaseEditFormFactory</v>
+      </c>
+      <c r="C39" t="str">
+        <f t="shared" si="9"/>
+        <v>public interface IIndebtnessInfoBaseEditFormFactory : ITypeEditorFormFactoryBase { }</v>
+      </c>
+      <c r="D39" t="str">
+        <f t="shared" si="10"/>
+        <v>IndebtnessInfoBase_Editor</v>
+      </c>
+      <c r="E39" t="str">
+        <f t="shared" si="11"/>
+        <v>public class IndebtnessInfoBase_Editor : GenericTypeEditor&lt;IndebtnessInfoBase&gt; { private IIndebtnessInfoBaseEditFormFactory _fact; protected override ITypeEditorFormFactoryBase TypeEditorFormFactory { get { if (_fact == null) _fact = TypeEditorsDispatcher.Container.Resolve&lt;IIndebtnessInfoBaseEditFormFactory&gt;(); return _fact; } }  }</v>
+      </c>
+      <c r="F39" t="str">
+        <f t="shared" si="12"/>
+        <v>IndebtnessInfoBaseEditFormFactoryBasic</v>
+      </c>
+      <c r="G39" t="str">
+        <f t="shared" si="13"/>
+        <v>public class IndebtnessInfoBaseEditFormFactoryBasic : IIndebtnessInfoBaseEditFormFactory { public System.Windows.Forms.Form SpawnInstance() { return new DummyForm&lt;IndebtnessInfoBase &gt;(); } }</v>
+      </c>
+      <c r="H39" t="str">
+        <f t="shared" si="14"/>
+        <v>cont.RegisterInstance&lt;IIndebtnessInfoBaseEditFormFactory&gt;(new IndebtnessInfoBaseEditFormFactoryBasic(), new ContainerControlledLifetimeManager());</v>
+      </c>
+      <c r="I39" t="str">
+        <f t="shared" si="15"/>
+        <v>[System.ComponentModel.Editor(typeof(BGU.DRPL.SignificantOwnership.Core.TypeEditors.IndebtnessInfoBase_Editor), typeof(System.Drawing.Design.UITypeEditor))]</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>57</v>
+      </c>
+      <c r="B40" t="str">
+        <f t="shared" si="8"/>
+        <v>ILiquidatedEntityOwnershipInfoEditFormFactory</v>
+      </c>
+      <c r="C40" t="str">
+        <f t="shared" si="9"/>
+        <v>public interface ILiquidatedEntityOwnershipInfoEditFormFactory : ITypeEditorFormFactoryBase { }</v>
+      </c>
+      <c r="D40" t="str">
+        <f t="shared" si="10"/>
+        <v>LiquidatedEntityOwnershipInfo_Editor</v>
+      </c>
+      <c r="E40" t="str">
+        <f t="shared" si="11"/>
+        <v>public class LiquidatedEntityOwnershipInfo_Editor : GenericTypeEditor&lt;LiquidatedEntityOwnershipInfo&gt; { private ILiquidatedEntityOwnershipInfoEditFormFactory _fact; protected override ITypeEditorFormFactoryBase TypeEditorFormFactory { get { if (_fact == null) _fact = TypeEditorsDispatcher.Container.Resolve&lt;ILiquidatedEntityOwnershipInfoEditFormFactory&gt;(); return _fact; } }  }</v>
+      </c>
+      <c r="F40" t="str">
+        <f t="shared" si="12"/>
+        <v>LiquidatedEntityOwnershipInfoEditFormFactoryBasic</v>
+      </c>
+      <c r="G40" t="str">
+        <f t="shared" si="13"/>
+        <v>public class LiquidatedEntityOwnershipInfoEditFormFactoryBasic : ILiquidatedEntityOwnershipInfoEditFormFactory { public System.Windows.Forms.Form SpawnInstance() { return new DummyForm&lt;LiquidatedEntityOwnershipInfo &gt;(); } }</v>
+      </c>
+      <c r="H40" t="str">
+        <f t="shared" si="14"/>
+        <v>cont.RegisterInstance&lt;ILiquidatedEntityOwnershipInfoEditFormFactory&gt;(new LiquidatedEntityOwnershipInfoEditFormFactoryBasic(), new ContainerControlledLifetimeManager());</v>
+      </c>
+      <c r="I40" t="str">
+        <f t="shared" si="15"/>
+        <v>[System.ComponentModel.Editor(typeof(BGU.DRPL.SignificantOwnership.Core.TypeEditors.LiquidatedEntityOwnershipInfo_Editor), typeof(System.Drawing.Design.UITypeEditor))]</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>58</v>
+      </c>
+      <c r="B41" t="str">
+        <f t="shared" si="8"/>
+        <v>ILoanInfoEditFormFactory</v>
+      </c>
+      <c r="C41" t="str">
+        <f t="shared" si="9"/>
+        <v>public interface ILoanInfoEditFormFactory : ITypeEditorFormFactoryBase { }</v>
+      </c>
+      <c r="D41" t="str">
+        <f t="shared" si="10"/>
+        <v>LoanInfo_Editor</v>
+      </c>
+      <c r="E41" t="str">
+        <f t="shared" si="11"/>
+        <v>public class LoanInfo_Editor : GenericTypeEditor&lt;LoanInfo&gt; { private ILoanInfoEditFormFactory _fact; protected override ITypeEditorFormFactoryBase TypeEditorFormFactory { get { if (_fact == null) _fact = TypeEditorsDispatcher.Container.Resolve&lt;ILoanInfoEditFormFactory&gt;(); return _fact; } }  }</v>
+      </c>
+      <c r="F41" t="str">
+        <f t="shared" si="12"/>
+        <v>LoanInfoEditFormFactoryBasic</v>
+      </c>
+      <c r="G41" t="str">
+        <f t="shared" si="13"/>
+        <v>public class LoanInfoEditFormFactoryBasic : ILoanInfoEditFormFactory { public System.Windows.Forms.Form SpawnInstance() { return new DummyForm&lt;LoanInfo &gt;(); } }</v>
+      </c>
+      <c r="H41" t="str">
+        <f t="shared" si="14"/>
+        <v>cont.RegisterInstance&lt;ILoanInfoEditFormFactory&gt;(new LoanInfoEditFormFactoryBasic(), new ContainerControlledLifetimeManager());</v>
+      </c>
+      <c r="I41" t="str">
+        <f t="shared" si="15"/>
+        <v>[System.ComponentModel.Editor(typeof(BGU.DRPL.SignificantOwnership.Core.TypeEditors.LoanInfo_Editor), typeof(System.Drawing.Design.UITypeEditor))]</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>59</v>
+      </c>
+      <c r="B42" t="str">
+        <f t="shared" si="8"/>
+        <v>IPaymentDeadlineInfoEditFormFactory</v>
+      </c>
+      <c r="C42" t="str">
+        <f t="shared" si="9"/>
+        <v>public interface IPaymentDeadlineInfoEditFormFactory : ITypeEditorFormFactoryBase { }</v>
+      </c>
+      <c r="D42" t="str">
+        <f t="shared" si="10"/>
+        <v>PaymentDeadlineInfo_Editor</v>
+      </c>
+      <c r="E42" t="str">
+        <f t="shared" si="11"/>
+        <v>public class PaymentDeadlineInfo_Editor : GenericTypeEditor&lt;PaymentDeadlineInfo&gt; { private IPaymentDeadlineInfoEditFormFactory _fact; protected override ITypeEditorFormFactoryBase TypeEditorFormFactory { get { if (_fact == null) _fact = TypeEditorsDispatcher.Container.Resolve&lt;IPaymentDeadlineInfoEditFormFactory&gt;(); return _fact; } }  }</v>
+      </c>
+      <c r="F42" t="str">
+        <f t="shared" si="12"/>
+        <v>PaymentDeadlineInfoEditFormFactoryBasic</v>
+      </c>
+      <c r="G42" t="str">
+        <f t="shared" si="13"/>
+        <v>public class PaymentDeadlineInfoEditFormFactoryBasic : IPaymentDeadlineInfoEditFormFactory { public System.Windows.Forms.Form SpawnInstance() { return new DummyForm&lt;PaymentDeadlineInfo &gt;(); } }</v>
+      </c>
+      <c r="H42" t="str">
+        <f t="shared" si="14"/>
+        <v>cont.RegisterInstance&lt;IPaymentDeadlineInfoEditFormFactory&gt;(new PaymentDeadlineInfoEditFormFactoryBasic(), new ContainerControlledLifetimeManager());</v>
+      </c>
+      <c r="I42" t="str">
+        <f t="shared" si="15"/>
+        <v>[System.ComponentModel.Editor(typeof(BGU.DRPL.SignificantOwnership.Core.TypeEditors.PaymentDeadlineInfo_Editor), typeof(System.Drawing.Design.UITypeEditor))]</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>60</v>
+      </c>
+      <c r="B43" t="str">
+        <f t="shared" si="8"/>
+        <v>IPaymentModeInfoEditFormFactory</v>
+      </c>
+      <c r="C43" t="str">
+        <f t="shared" si="9"/>
+        <v>public interface IPaymentModeInfoEditFormFactory : ITypeEditorFormFactoryBase { }</v>
+      </c>
+      <c r="D43" t="str">
+        <f t="shared" si="10"/>
+        <v>PaymentModeInfo_Editor</v>
+      </c>
+      <c r="E43" t="str">
+        <f t="shared" si="11"/>
+        <v>public class PaymentModeInfo_Editor : GenericTypeEditor&lt;PaymentModeInfo&gt; { private IPaymentModeInfoEditFormFactory _fact; protected override ITypeEditorFormFactoryBase TypeEditorFormFactory { get { if (_fact == null) _fact = TypeEditorsDispatcher.Container.Resolve&lt;IPaymentModeInfoEditFormFactory&gt;(); return _fact; } }  }</v>
+      </c>
+      <c r="F43" t="str">
+        <f t="shared" si="12"/>
+        <v>PaymentModeInfoEditFormFactoryBasic</v>
+      </c>
+      <c r="G43" t="str">
+        <f t="shared" si="13"/>
+        <v>public class PaymentModeInfoEditFormFactoryBasic : IPaymentModeInfoEditFormFactory { public System.Windows.Forms.Form SpawnInstance() { return new DummyForm&lt;PaymentModeInfo &gt;(); } }</v>
+      </c>
+      <c r="H43" t="str">
+        <f t="shared" si="14"/>
+        <v>cont.RegisterInstance&lt;IPaymentModeInfoEditFormFactory&gt;(new PaymentModeInfoEditFormFactoryBasic(), new ContainerControlledLifetimeManager());</v>
+      </c>
+      <c r="I43" t="str">
+        <f t="shared" si="15"/>
+        <v>[System.ComponentModel.Editor(typeof(BGU.DRPL.SignificantOwnership.Core.TypeEditors.PaymentModeInfo_Editor), typeof(System.Drawing.Design.UITypeEditor))]</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>61</v>
+      </c>
+      <c r="B44" t="str">
+        <f t="shared" si="8"/>
+        <v>IProfessionLicenseInfoEditFormFactory</v>
+      </c>
+      <c r="C44" t="str">
+        <f t="shared" si="9"/>
+        <v>public interface IProfessionLicenseInfoEditFormFactory : ITypeEditorFormFactoryBase { }</v>
+      </c>
+      <c r="D44" t="str">
+        <f t="shared" si="10"/>
+        <v>ProfessionLicenseInfo_Editor</v>
+      </c>
+      <c r="E44" t="str">
+        <f t="shared" si="11"/>
+        <v>public class ProfessionLicenseInfo_Editor : GenericTypeEditor&lt;ProfessionLicenseInfo&gt; { private IProfessionLicenseInfoEditFormFactory _fact; protected override ITypeEditorFormFactoryBase TypeEditorFormFactory { get { if (_fact == null) _fact = TypeEditorsDispatcher.Container.Resolve&lt;IProfessionLicenseInfoEditFormFactory&gt;(); return _fact; } }  }</v>
+      </c>
+      <c r="F44" t="str">
+        <f t="shared" si="12"/>
+        <v>ProfessionLicenseInfoEditFormFactoryBasic</v>
+      </c>
+      <c r="G44" t="str">
+        <f t="shared" si="13"/>
+        <v>public class ProfessionLicenseInfoEditFormFactoryBasic : IProfessionLicenseInfoEditFormFactory { public System.Windows.Forms.Form SpawnInstance() { return new DummyForm&lt;ProfessionLicenseInfo &gt;(); } }</v>
+      </c>
+      <c r="H44" t="str">
+        <f t="shared" si="14"/>
+        <v>cont.RegisterInstance&lt;IProfessionLicenseInfoEditFormFactory&gt;(new ProfessionLicenseInfoEditFormFactoryBasic(), new ContainerControlledLifetimeManager());</v>
+      </c>
+      <c r="I44" t="str">
+        <f t="shared" si="15"/>
+        <v>[System.ComponentModel.Editor(typeof(BGU.DRPL.SignificantOwnership.Core.TypeEditors.ProfessionLicenseInfo_Editor), typeof(System.Drawing.Design.UITypeEditor))]</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>62</v>
+      </c>
+      <c r="B45" t="str">
+        <f t="shared" si="8"/>
+        <v>ISharesAcquisitionInfoEditFormFactory</v>
+      </c>
+      <c r="C45" t="str">
+        <f t="shared" si="9"/>
+        <v>public interface ISharesAcquisitionInfoEditFormFactory : ITypeEditorFormFactoryBase { }</v>
+      </c>
+      <c r="D45" t="str">
+        <f t="shared" si="10"/>
+        <v>SharesAcquisitionInfo_Editor</v>
+      </c>
+      <c r="E45" t="str">
+        <f t="shared" si="11"/>
+        <v>public class SharesAcquisitionInfo_Editor : GenericTypeEditor&lt;SharesAcquisitionInfo&gt; { private ISharesAcquisitionInfoEditFormFactory _fact; protected override ITypeEditorFormFactoryBase TypeEditorFormFactory { get { if (_fact == null) _fact = TypeEditorsDispatcher.Container.Resolve&lt;ISharesAcquisitionInfoEditFormFactory&gt;(); return _fact; } }  }</v>
+      </c>
+      <c r="F45" t="str">
+        <f t="shared" si="12"/>
+        <v>SharesAcquisitionInfoEditFormFactoryBasic</v>
+      </c>
+      <c r="G45" t="str">
+        <f t="shared" si="13"/>
+        <v>public class SharesAcquisitionInfoEditFormFactoryBasic : ISharesAcquisitionInfoEditFormFactory { public System.Windows.Forms.Form SpawnInstance() { return new DummyForm&lt;SharesAcquisitionInfo &gt;(); } }</v>
+      </c>
+      <c r="H45" t="str">
+        <f t="shared" si="14"/>
+        <v>cont.RegisterInstance&lt;ISharesAcquisitionInfoEditFormFactory&gt;(new SharesAcquisitionInfoEditFormFactoryBasic(), new ContainerControlledLifetimeManager());</v>
+      </c>
+      <c r="I45" t="str">
+        <f t="shared" si="15"/>
+        <v>[System.ComponentModel.Editor(typeof(BGU.DRPL.SignificantOwnership.Core.TypeEditors.SharesAcquisitionInfo_Editor), typeof(System.Drawing.Design.UITypeEditor))]</v>
+      </c>
+    </row>
+    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>63</v>
+      </c>
+      <c r="B46" t="str">
+        <f t="shared" si="8"/>
+        <v>IBankAccountInfoEditFormFactory</v>
+      </c>
+      <c r="C46" t="str">
+        <f t="shared" si="9"/>
+        <v>public interface IBankAccountInfoEditFormFactory : ITypeEditorFormFactoryBase { }</v>
+      </c>
+      <c r="D46" t="str">
+        <f t="shared" si="10"/>
+        <v>BankAccountInfo_Editor</v>
+      </c>
+      <c r="E46" t="str">
+        <f t="shared" si="11"/>
+        <v>public class BankAccountInfo_Editor : GenericTypeEditor&lt;BankAccountInfo&gt; { private IBankAccountInfoEditFormFactory _fact; protected override ITypeEditorFormFactoryBase TypeEditorFormFactory { get { if (_fact == null) _fact = TypeEditorsDispatcher.Container.Resolve&lt;IBankAccountInfoEditFormFactory&gt;(); return _fact; } }  }</v>
+      </c>
+      <c r="F46" t="str">
+        <f t="shared" si="12"/>
+        <v>BankAccountInfoEditFormFactoryBasic</v>
+      </c>
+      <c r="G46" t="str">
+        <f t="shared" si="13"/>
+        <v>public class BankAccountInfoEditFormFactoryBasic : IBankAccountInfoEditFormFactory { public System.Windows.Forms.Form SpawnInstance() { return new DummyForm&lt;BankAccountInfo &gt;(); } }</v>
+      </c>
+      <c r="H46" t="str">
+        <f t="shared" si="14"/>
+        <v>cont.RegisterInstance&lt;IBankAccountInfoEditFormFactory&gt;(new BankAccountInfoEditFormFactoryBasic(), new ContainerControlledLifetimeManager());</v>
+      </c>
+      <c r="I46" t="str">
+        <f t="shared" si="15"/>
+        <v>[System.ComponentModel.Editor(typeof(BGU.DRPL.SignificantOwnership.Core.TypeEditors.BankAccountInfo_Editor), typeof(System.Drawing.Design.UITypeEditor))]</v>
+      </c>
+    </row>
+    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>64</v>
+      </c>
+      <c r="B47" t="str">
+        <f t="shared" si="8"/>
+        <v>IProfessionLicensingBodyInfoEditFormFactory</v>
+      </c>
+      <c r="C47" t="str">
+        <f t="shared" si="9"/>
+        <v>public interface IProfessionLicensingBodyInfoEditFormFactory : ITypeEditorFormFactoryBase { }</v>
+      </c>
+      <c r="D47" t="str">
+        <f t="shared" si="10"/>
+        <v>ProfessionLicensingBodyInfo_Editor</v>
+      </c>
+      <c r="E47" t="str">
+        <f t="shared" si="11"/>
+        <v>public class ProfessionLicensingBodyInfo_Editor : GenericTypeEditor&lt;ProfessionLicensingBodyInfo&gt; { private IProfessionLicensingBodyInfoEditFormFactory _fact; protected override ITypeEditorFormFactoryBase TypeEditorFormFactory { get { if (_fact == null) _fact = TypeEditorsDispatcher.Container.Resolve&lt;IProfessionLicensingBodyInfoEditFormFactory&gt;(); return _fact; } }  }</v>
+      </c>
+      <c r="F47" t="str">
+        <f t="shared" si="12"/>
+        <v>ProfessionLicensingBodyInfoEditFormFactoryBasic</v>
+      </c>
+      <c r="G47" t="str">
+        <f t="shared" si="13"/>
+        <v>public class ProfessionLicensingBodyInfoEditFormFactoryBasic : IProfessionLicensingBodyInfoEditFormFactory { public System.Windows.Forms.Form SpawnInstance() { return new DummyForm&lt;ProfessionLicensingBodyInfo &gt;(); } }</v>
+      </c>
+      <c r="H47" t="str">
+        <f t="shared" si="14"/>
+        <v>cont.RegisterInstance&lt;IProfessionLicensingBodyInfoEditFormFactory&gt;(new ProfessionLicensingBodyInfoEditFormFactoryBasic(), new ContainerControlledLifetimeManager());</v>
+      </c>
+      <c r="I47" t="str">
+        <f t="shared" si="15"/>
+        <v>[System.ComponentModel.Editor(typeof(BGU.DRPL.SignificantOwnership.Core.TypeEditors.ProfessionLicensingBodyInfo_Editor), typeof(System.Drawing.Design.UITypeEditor))]</v>
+      </c>
+    </row>
+    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>65</v>
+      </c>
+      <c r="B48" t="str">
+        <f t="shared" si="8"/>
+        <v>IPublicationInfoEditFormFactory</v>
+      </c>
+      <c r="C48" t="str">
+        <f t="shared" si="9"/>
+        <v>public interface IPublicationInfoEditFormFactory : ITypeEditorFormFactoryBase { }</v>
+      </c>
+      <c r="D48" t="str">
+        <f t="shared" si="10"/>
+        <v>PublicationInfo_Editor</v>
+      </c>
+      <c r="E48" t="str">
+        <f t="shared" si="11"/>
+        <v>public class PublicationInfo_Editor : GenericTypeEditor&lt;PublicationInfo&gt; { private IPublicationInfoEditFormFactory _fact; protected override ITypeEditorFormFactoryBase TypeEditorFormFactory { get { if (_fact == null) _fact = TypeEditorsDispatcher.Container.Resolve&lt;IPublicationInfoEditFormFactory&gt;(); return _fact; } }  }</v>
+      </c>
+      <c r="F48" t="str">
+        <f t="shared" si="12"/>
+        <v>PublicationInfoEditFormFactoryBasic</v>
+      </c>
+      <c r="G48" t="str">
+        <f t="shared" si="13"/>
+        <v>public class PublicationInfoEditFormFactoryBasic : IPublicationInfoEditFormFactory { public System.Windows.Forms.Form SpawnInstance() { return new DummyForm&lt;PublicationInfo &gt;(); } }</v>
+      </c>
+      <c r="H48" t="str">
+        <f t="shared" si="14"/>
+        <v>cont.RegisterInstance&lt;IPublicationInfoEditFormFactory&gt;(new PublicationInfoEditFormFactoryBasic(), new ContainerControlledLifetimeManager());</v>
+      </c>
+      <c r="I48" t="str">
+        <f t="shared" si="15"/>
+        <v>[System.ComponentModel.Editor(typeof(BGU.DRPL.SignificantOwnership.Core.TypeEditors.PublicationInfo_Editor), typeof(System.Drawing.Design.UITypeEditor))]</v>
+      </c>
+    </row>
+    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>66</v>
+      </c>
+      <c r="B49" t="str">
+        <f t="shared" si="8"/>
+        <v>IPublishingHouseInfoEditFormFactory</v>
+      </c>
+      <c r="C49" t="str">
+        <f t="shared" si="9"/>
+        <v>public interface IPublishingHouseInfoEditFormFactory : ITypeEditorFormFactoryBase { }</v>
+      </c>
+      <c r="D49" t="str">
+        <f t="shared" si="10"/>
+        <v>PublishingHouseInfo_Editor</v>
+      </c>
+      <c r="E49" t="str">
+        <f t="shared" si="11"/>
+        <v>public class PublishingHouseInfo_Editor : GenericTypeEditor&lt;PublishingHouseInfo&gt; { private IPublishingHouseInfoEditFormFactory _fact; protected override ITypeEditorFormFactoryBase TypeEditorFormFactory { get { if (_fact == null) _fact = TypeEditorsDispatcher.Container.Resolve&lt;IPublishingHouseInfoEditFormFactory&gt;(); return _fact; } }  }</v>
+      </c>
+      <c r="F49" t="str">
+        <f t="shared" si="12"/>
+        <v>PublishingHouseInfoEditFormFactoryBasic</v>
+      </c>
+      <c r="G49" t="str">
+        <f t="shared" si="13"/>
+        <v>public class PublishingHouseInfoEditFormFactoryBasic : IPublishingHouseInfoEditFormFactory { public System.Windows.Forms.Form SpawnInstance() { return new DummyForm&lt;PublishingHouseInfo &gt;(); } }</v>
+      </c>
+      <c r="H49" t="str">
+        <f t="shared" si="14"/>
+        <v>cont.RegisterInstance&lt;IPublishingHouseInfoEditFormFactory&gt;(new PublishingHouseInfoEditFormFactoryBasic(), new ContainerControlledLifetimeManager());</v>
+      </c>
+      <c r="I49" t="str">
+        <f t="shared" si="15"/>
+        <v>[System.ComponentModel.Editor(typeof(BGU.DRPL.SignificantOwnership.Core.TypeEditors.PublishingHouseInfo_Editor), typeof(System.Drawing.Design.UITypeEditor))]</v>
+      </c>
+    </row>
+    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>67</v>
+      </c>
+      <c r="B50" t="str">
+        <f t="shared" si="8"/>
+        <v>IUniversityOrCollegeInfoEditFormFactory</v>
+      </c>
+      <c r="C50" t="str">
+        <f t="shared" si="9"/>
+        <v>public interface IUniversityOrCollegeInfoEditFormFactory : ITypeEditorFormFactoryBase { }</v>
+      </c>
+      <c r="D50" t="str">
+        <f t="shared" si="10"/>
+        <v>UniversityOrCollegeInfo_Editor</v>
+      </c>
+      <c r="E50" t="str">
+        <f t="shared" si="11"/>
+        <v>public class UniversityOrCollegeInfo_Editor : GenericTypeEditor&lt;UniversityOrCollegeInfo&gt; { private IUniversityOrCollegeInfoEditFormFactory _fact; protected override ITypeEditorFormFactoryBase TypeEditorFormFactory { get { if (_fact == null) _fact = TypeEditorsDispatcher.Container.Resolve&lt;IUniversityOrCollegeInfoEditFormFactory&gt;(); return _fact; } }  }</v>
+      </c>
+      <c r="F50" t="str">
+        <f t="shared" si="12"/>
+        <v>UniversityOrCollegeInfoEditFormFactoryBasic</v>
+      </c>
+      <c r="G50" t="str">
+        <f t="shared" si="13"/>
+        <v>public class UniversityOrCollegeInfoEditFormFactoryBasic : IUniversityOrCollegeInfoEditFormFactory { public System.Windows.Forms.Form SpawnInstance() { return new DummyForm&lt;UniversityOrCollegeInfo &gt;(); } }</v>
+      </c>
+      <c r="H50" t="str">
+        <f t="shared" si="14"/>
+        <v>cont.RegisterInstance&lt;IUniversityOrCollegeInfoEditFormFactory&gt;(new UniversityOrCollegeInfoEditFormFactoryBasic(), new ContainerControlledLifetimeManager());</v>
+      </c>
+      <c r="I50" t="str">
+        <f t="shared" si="15"/>
+        <v>[System.ComponentModel.Editor(typeof(BGU.DRPL.SignificantOwnership.Core.TypeEditors.UniversityOrCollegeInfo_Editor), typeof(System.Drawing.Design.UITypeEditor))]</v>
+      </c>
+    </row>
+    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>68</v>
+      </c>
+      <c r="B51" t="str">
+        <f t="shared" ref="B51" si="16">"I"&amp; TRIM(A51) &amp; "EditFormFactory"</f>
+        <v>IFinancialOversightAuthorityInfoEditFormFactory</v>
+      </c>
+      <c r="C51" t="str">
+        <f t="shared" ref="C51" si="17">"public interface I"&amp; TRIM(A51) &amp; "EditFormFactory : ITypeEditorFormFactoryBase { }"</f>
+        <v>public interface IFinancialOversightAuthorityInfoEditFormFactory : ITypeEditorFormFactoryBase { }</v>
+      </c>
+      <c r="D51" t="str">
+        <f t="shared" ref="D51" si="18">A51&amp; "_Editor"</f>
+        <v>FinancialOversightAuthorityInfo_Editor</v>
+      </c>
+      <c r="E51" t="str">
+        <f t="shared" ref="E51" si="19">"public class " &amp; D51 &amp; " : GenericTypeEditor&lt;"&amp;A51&amp;"&gt; { private " &amp; B51 &amp; " _fact; protected override ITypeEditorFormFactoryBase TypeEditorFormFactory { get { if (_fact == null) _fact = TypeEditorsDispatcher.Container.Resolve&lt;" &amp;B51 &amp; "&gt;(); return _fact; } }  }"</f>
+        <v>public class FinancialOversightAuthorityInfo_Editor : GenericTypeEditor&lt;FinancialOversightAuthorityInfo&gt; { private IFinancialOversightAuthorityInfoEditFormFactory _fact; protected override ITypeEditorFormFactoryBase TypeEditorFormFactory { get { if (_fact == null) _fact = TypeEditorsDispatcher.Container.Resolve&lt;IFinancialOversightAuthorityInfoEditFormFactory&gt;(); return _fact; } }  }</v>
+      </c>
+      <c r="F51" t="str">
+        <f t="shared" ref="F51" si="20">A51&amp; "EditFormFactoryBasic"</f>
+        <v>FinancialOversightAuthorityInfoEditFormFactoryBasic</v>
+      </c>
+      <c r="G51" t="str">
+        <f t="shared" ref="G51" si="21">"public class " &amp;F51&amp; " : " &amp; B51 &amp; " { public System.Windows.Forms.Form SpawnInstance() { return new DummyForm&lt;" &amp;A51&amp; " &gt;(); } }"</f>
+        <v>public class FinancialOversightAuthorityInfoEditFormFactoryBasic : IFinancialOversightAuthorityInfoEditFormFactory { public System.Windows.Forms.Form SpawnInstance() { return new DummyForm&lt;FinancialOversightAuthorityInfo &gt;(); } }</v>
+      </c>
+      <c r="H51" t="str">
+        <f t="shared" ref="H51" si="22">"cont.RegisterInstance&lt;" &amp; B51 &amp; "&gt;(new " &amp; F51 &amp; "(), new ContainerControlledLifetimeManager());"</f>
+        <v>cont.RegisterInstance&lt;IFinancialOversightAuthorityInfoEditFormFactory&gt;(new FinancialOversightAuthorityInfoEditFormFactoryBasic(), new ContainerControlledLifetimeManager());</v>
+      </c>
+      <c r="I51" t="str">
+        <f t="shared" ref="I51" si="23">"[System.ComponentModel.Editor(typeof(BGU.DRPL.SignificantOwnership.Core.TypeEditors." &amp;D51 &amp; "), typeof(System.Drawing.Design.UITypeEditor))]"</f>
+        <v>[System.ComponentModel.Editor(typeof(BGU.DRPL.SignificantOwnership.Core.TypeEditors.FinancialOversightAuthorityInfo_Editor), typeof(System.Drawing.Design.UITypeEditor))]</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>